<commit_message>
add Climb exel to MATLAB file
</commit_message>
<xml_diff>
--- a/Matching Diagram/Climb.xlsx
+++ b/Matching Diagram/Climb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\Airplane-Design-II\Matching Diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7FCDB85-A87E-4A32-BDFF-A51EC127A118}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54B6086-E378-4EEC-A08A-2905F150493E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="6" xr2:uid="{90B7881E-F26A-4004-B09D-A06CC16A62D7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{90B7881E-F26A-4004-B09D-A06CC16A62D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="58">
   <si>
     <t>وضعیت</t>
   </si>
@@ -212,6 +212,9 @@
   </si>
   <si>
     <t>121 open Landing gear</t>
+  </si>
+  <si>
+    <t>AOE</t>
   </si>
 </sst>
 </file>
@@ -734,28 +737,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -770,6 +767,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -782,26 +794,17 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -8442,7 +8445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AC84584-1541-4318-9FBD-F89612D9C3B7}">
   <dimension ref="A1:W84"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
@@ -8495,7 +8498,7 @@
       <c r="B3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="61" t="s">
+      <c r="C3" s="44" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="11">
@@ -8510,7 +8513,7 @@
       <c r="M3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="48" t="s">
+      <c r="N3" s="42" t="s">
         <v>3</v>
       </c>
       <c r="O3" s="11">
@@ -8521,7 +8524,7 @@
       <c r="B4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="62"/>
+      <c r="C4" s="45"/>
       <c r="D4" s="11">
         <v>0.5</v>
       </c>
@@ -8534,7 +8537,7 @@
       <c r="M4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="N4" s="48"/>
+      <c r="N4" s="42"/>
       <c r="O4" s="11">
         <v>0.02</v>
       </c>
@@ -8543,14 +8546,14 @@
       <c r="B5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="63"/>
+      <c r="C5" s="46"/>
       <c r="D5" s="11">
         <v>0.48</v>
       </c>
       <c r="M5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="N5" s="48"/>
+      <c r="N5" s="42"/>
       <c r="O5" s="11">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -8559,7 +8562,7 @@
       <c r="B6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="61" t="s">
+      <c r="C6" s="44" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="11">
@@ -8580,7 +8583,7 @@
       <c r="M6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="N6" s="48"/>
+      <c r="N6" s="42"/>
       <c r="O6" s="11">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -8589,7 +8592,7 @@
       <c r="B7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="62"/>
+      <c r="C7" s="45"/>
       <c r="D7" s="11">
         <v>0.53</v>
       </c>
@@ -8608,7 +8611,7 @@
       <c r="M7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="N7" s="48" t="s">
+      <c r="N7" s="42" t="s">
         <v>6</v>
       </c>
       <c r="O7" s="11">
@@ -8619,7 +8622,7 @@
       <c r="B8" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="63"/>
+      <c r="C8" s="46"/>
       <c r="D8" s="11">
         <v>0.51</v>
       </c>
@@ -8638,7 +8641,7 @@
       <c r="M8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="N8" s="48"/>
+      <c r="N8" s="42"/>
       <c r="O8" s="11">
         <v>1.4999999999999999E-2</v>
       </c>
@@ -8647,7 +8650,7 @@
       <c r="B9" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="61" t="s">
+      <c r="C9" s="44" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="11">
@@ -8668,7 +8671,7 @@
       <c r="M9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="N9" s="48"/>
+      <c r="N9" s="42"/>
       <c r="O9" s="11">
         <v>6.5000000000000002E-2</v>
       </c>
@@ -8677,14 +8680,14 @@
       <c r="B10" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="62"/>
+      <c r="C10" s="45"/>
       <c r="D10" s="11">
         <v>0.59</v>
       </c>
       <c r="M10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="N10" s="48"/>
+      <c r="N10" s="42"/>
       <c r="O10" s="11">
         <v>0.02</v>
       </c>
@@ -8693,14 +8696,14 @@
       <c r="B11" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="64"/>
+      <c r="C11" s="47"/>
       <c r="D11" s="13">
         <v>0.54</v>
       </c>
       <c r="M11" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="N11" s="48" t="s">
+      <c r="N11" s="42" t="s">
         <v>7</v>
       </c>
       <c r="O11" s="11">
@@ -8711,7 +8714,7 @@
       <c r="M12" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="N12" s="48"/>
+      <c r="N12" s="42"/>
       <c r="O12" s="11">
         <v>0.01</v>
       </c>
@@ -8720,7 +8723,7 @@
       <c r="M13" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="N13" s="48"/>
+      <c r="N13" s="42"/>
       <c r="O13" s="11">
         <v>5.5E-2</v>
       </c>
@@ -8729,7 +8732,7 @@
       <c r="M14" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="N14" s="49"/>
+      <c r="N14" s="43"/>
       <c r="O14" s="13">
         <v>1.4999999999999999E-2</v>
       </c>
@@ -8741,33 +8744,33 @@
       <c r="E18" s="34"/>
     </row>
     <row r="19" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C19" s="47" t="s">
+      <c r="C19" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="47"/>
+      <c r="D19" s="53"/>
       <c r="E19" s="35"/>
-      <c r="F19" s="47" t="s">
+      <c r="F19" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="G19" s="47"/>
-      <c r="I19" s="47" t="s">
+      <c r="G19" s="53"/>
+      <c r="I19" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="J19" s="47"/>
-      <c r="M19" s="54" t="s">
+      <c r="J19" s="53"/>
+      <c r="M19" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="N19" s="55"/>
-      <c r="O19" s="55"/>
-      <c r="P19" s="55"/>
-      <c r="Q19" s="55"/>
-      <c r="S19" s="56" t="s">
+      <c r="N19" s="58"/>
+      <c r="O19" s="58"/>
+      <c r="P19" s="58"/>
+      <c r="Q19" s="58"/>
+      <c r="S19" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="T19" s="57"/>
-      <c r="U19" s="57"/>
-      <c r="V19" s="57"/>
-      <c r="W19" s="57"/>
+      <c r="T19" s="60"/>
+      <c r="U19" s="60"/>
+      <c r="V19" s="60"/>
+      <c r="W19" s="60"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C20" s="16" t="s">
@@ -8789,10 +8792,10 @@
       <c r="J20" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="M20" s="58" t="s">
+      <c r="M20" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="N20" s="59"/>
+      <c r="N20" s="55"/>
       <c r="O20" s="28" t="s">
         <v>1</v>
       </c>
@@ -8802,10 +8805,10 @@
       <c r="Q20" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="S20" s="58" t="s">
+      <c r="S20" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="T20" s="59"/>
+      <c r="T20" s="55"/>
       <c r="U20" s="28" t="s">
         <v>1</v>
       </c>
@@ -8839,11 +8842,11 @@
         <f>1/(3.14*$D$4*$B$33)</f>
         <v>6.7046597385182705E-2</v>
       </c>
-      <c r="M21" s="50" t="s">
+      <c r="M21" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="N21" s="51"/>
-      <c r="O21" s="48" t="s">
+      <c r="N21" s="49"/>
+      <c r="O21" s="42" t="s">
         <v>3</v>
       </c>
       <c r="P21" s="24">
@@ -8854,11 +8857,11 @@
         <f>G27/P21</f>
         <v>7.9758895915499473</v>
       </c>
-      <c r="S21" s="50" t="s">
+      <c r="S21" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="T21" s="51"/>
-      <c r="U21" s="48" t="s">
+      <c r="T21" s="49"/>
+      <c r="U21" s="42" t="s">
         <v>3</v>
       </c>
       <c r="V21" s="24">
@@ -8893,11 +8896,11 @@
         <f>1/(3.14*$D$7*$B$33)</f>
         <v>6.3251506967153495E-2</v>
       </c>
-      <c r="M22" s="50" t="s">
+      <c r="M22" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="N22" s="51"/>
-      <c r="O22" s="48"/>
+      <c r="N22" s="49"/>
+      <c r="O22" s="42"/>
       <c r="P22" s="24">
         <f>$G$3+$G$21*$G$27^2+$O$5</f>
         <v>0.22064662010569813</v>
@@ -8906,11 +8909,11 @@
         <f>G27/P22</f>
         <v>6.1684996601453355</v>
       </c>
-      <c r="S22" s="50" t="s">
+      <c r="S22" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="T22" s="51"/>
-      <c r="U22" s="48"/>
+      <c r="T22" s="49"/>
+      <c r="U22" s="42"/>
       <c r="V22" s="24">
         <f>$G$4+$G$21*$G$27^2+$O$5</f>
         <v>0.22215962010569812</v>
@@ -8942,11 +8945,11 @@
         <f>1/(3.14*$D$10*$B$33)</f>
         <v>5.6819150326426024E-2</v>
       </c>
-      <c r="M23" s="50" t="s">
+      <c r="M23" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="N23" s="51"/>
-      <c r="O23" s="48"/>
+      <c r="N23" s="49"/>
+      <c r="O23" s="42"/>
       <c r="P23" s="24">
         <f>$G$3+$J$21*$J$27^2+$O$4</f>
         <v>0.15350094406534229</v>
@@ -8955,11 +8958,11 @@
         <f>J27/P23</f>
         <v>8.6143707951652342</v>
       </c>
-      <c r="S23" s="50" t="s">
+      <c r="S23" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="T23" s="51"/>
-      <c r="U23" s="48"/>
+      <c r="T23" s="49"/>
+      <c r="U23" s="42"/>
       <c r="V23" s="24">
         <f>$G$3+$J$21*$J$27^2+$O$4</f>
         <v>0.15350094406534229</v>
@@ -8970,11 +8973,11 @@
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="M24" s="50" t="s">
+      <c r="M24" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="N24" s="51"/>
-      <c r="O24" s="48" t="s">
+      <c r="N24" s="49"/>
+      <c r="O24" s="42" t="s">
         <v>6</v>
       </c>
       <c r="P24" s="24">
@@ -8985,11 +8988,11 @@
         <f>G28/P24</f>
         <v>6.5805637550161364</v>
       </c>
-      <c r="S24" s="50" t="s">
+      <c r="S24" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="T24" s="51"/>
-      <c r="U24" s="48" t="s">
+      <c r="T24" s="49"/>
+      <c r="U24" s="42" t="s">
         <v>6</v>
       </c>
       <c r="V24" s="24">
@@ -9002,23 +9005,23 @@
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C25" s="47" t="s">
+      <c r="C25" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="47"/>
-      <c r="F25" s="47" t="s">
+      <c r="D25" s="53"/>
+      <c r="F25" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="G25" s="47"/>
-      <c r="I25" s="47" t="s">
+      <c r="G25" s="53"/>
+      <c r="I25" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="J25" s="47"/>
-      <c r="M25" s="50" t="s">
+      <c r="J25" s="53"/>
+      <c r="M25" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="N25" s="51"/>
-      <c r="O25" s="48"/>
+      <c r="N25" s="49"/>
+      <c r="O25" s="42"/>
       <c r="P25" s="24">
         <f>$G$3+$G$22*$G$28^2+$O$9</f>
         <v>0.35524513669441948</v>
@@ -9027,11 +9030,11 @@
         <f>G28/P25</f>
         <v>5.7469833948986322</v>
       </c>
-      <c r="S25" s="50" t="s">
+      <c r="S25" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="T25" s="51"/>
-      <c r="U25" s="48"/>
+      <c r="T25" s="49"/>
+      <c r="U25" s="42"/>
       <c r="V25" s="24">
         <f>$G$4+$G$22*$G$28^2+$O$9</f>
         <v>0.35675813669441953</v>
@@ -9060,11 +9063,11 @@
       <c r="J26" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="M26" s="50" t="s">
+      <c r="M26" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="N26" s="51"/>
-      <c r="O26" s="48"/>
+      <c r="N26" s="49"/>
+      <c r="O26" s="42"/>
       <c r="P26" s="24">
         <f>$G$3+$J$22*$J$28^2+$O$8</f>
         <v>0.24036489080050738</v>
@@ -9073,11 +9076,11 @@
         <f>J28/P26</f>
         <v>7.5642570432253002</v>
       </c>
-      <c r="S26" s="50" t="s">
+      <c r="S26" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="T26" s="51"/>
-      <c r="U26" s="48"/>
+      <c r="T26" s="49"/>
+      <c r="U26" s="42"/>
       <c r="V26" s="24">
         <f>$G$4+$J$22*$J$28^2+$O$8</f>
         <v>0.24187789080050737</v>
@@ -9109,11 +9112,11 @@
         <f>I7/$B$32^2</f>
         <v>1.3223140495867767</v>
       </c>
-      <c r="M27" s="50" t="s">
+      <c r="M27" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="N27" s="51"/>
-      <c r="O27" s="48" t="s">
+      <c r="N27" s="49"/>
+      <c r="O27" s="42" t="s">
         <v>7</v>
       </c>
       <c r="P27" s="24">
@@ -9124,11 +9127,11 @@
         <f>G29/P27</f>
         <v>6.8396962760703239</v>
       </c>
-      <c r="S27" s="50" t="s">
+      <c r="S27" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="T27" s="51"/>
-      <c r="U27" s="48" t="s">
+      <c r="T27" s="49"/>
+      <c r="U27" s="42" t="s">
         <v>7</v>
       </c>
       <c r="V27" s="24">
@@ -9162,11 +9165,11 @@
         <f>I8/$B$32^2</f>
         <v>1.8181818181818181</v>
       </c>
-      <c r="M28" s="50" t="s">
+      <c r="M28" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="N28" s="51"/>
-      <c r="O28" s="48"/>
+      <c r="N28" s="49"/>
+      <c r="O28" s="42"/>
       <c r="P28" s="24">
         <f>$G$3+$G$23*$G$29^2+$O$13</f>
         <v>0.34954624050169353</v>
@@ -9175,11 +9178,11 @@
         <f>G29/P28</f>
         <v>6.0570019731645335</v>
       </c>
-      <c r="S28" s="50" t="s">
+      <c r="S28" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="T28" s="51"/>
-      <c r="U28" s="48"/>
+      <c r="T28" s="49"/>
+      <c r="U28" s="42"/>
       <c r="V28" s="24">
         <f>$G$4+$G$23*$G$29^2+$O$13</f>
         <v>0.35105924050169357</v>
@@ -9211,11 +9214,11 @@
         <f>I9/$B$32^2</f>
         <v>1.8181818181818181</v>
       </c>
-      <c r="M29" s="52" t="s">
+      <c r="M29" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="N29" s="53"/>
-      <c r="O29" s="49"/>
+      <c r="N29" s="51"/>
+      <c r="O29" s="43"/>
       <c r="P29" s="27">
         <f>$G$3+$J$23*$J$29^2+$O$12</f>
         <v>0.21410090190554057</v>
@@ -9224,11 +9227,11 @@
         <f>J29/P29</f>
         <v>8.4921726251484166</v>
       </c>
-      <c r="S29" s="52" t="s">
+      <c r="S29" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="T29" s="53"/>
-      <c r="U29" s="49"/>
+      <c r="T29" s="51"/>
+      <c r="U29" s="43"/>
       <c r="V29" s="27">
         <f>$G$4+$J$23*$J$29^2+$O$12</f>
         <v>0.21561390190554056</v>
@@ -9256,10 +9259,10 @@
       <c r="B31">
         <v>1.1499999999999999</v>
       </c>
-      <c r="M31" s="60" t="s">
+      <c r="M31" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="N31" s="60"/>
+      <c r="N31" s="52"/>
       <c r="O31" s="16" t="s">
         <v>22</v>
       </c>
@@ -9331,11 +9334,11 @@
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A34" s="46" t="s">
+      <c r="A34" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="46"/>
-      <c r="C34" s="46"/>
+      <c r="B34" s="56"/>
+      <c r="C34" s="56"/>
       <c r="D34" s="31"/>
       <c r="O34" s="17" t="s">
         <v>27</v>
@@ -9417,11 +9420,11 @@
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A42" s="46" t="s">
+      <c r="A42" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="46"/>
-      <c r="C42" s="46"/>
+      <c r="B42" s="56"/>
+      <c r="C42" s="56"/>
       <c r="D42" s="31"/>
       <c r="E42" t="s">
         <v>48</v>
@@ -9487,11 +9490,11 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="46" t="s">
+      <c r="A50" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="B50" s="46"/>
-      <c r="C50" s="46"/>
+      <c r="B50" s="56"/>
+      <c r="C50" s="56"/>
       <c r="D50" s="31"/>
       <c r="E50" t="s">
         <v>49</v>
@@ -9557,16 +9560,16 @@
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C57" s="42" t="s">
+      <c r="C57" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="D57" s="42"/>
-      <c r="E57" s="42"/>
-      <c r="F57" s="42" t="s">
+      <c r="D57" s="61"/>
+      <c r="E57" s="61"/>
+      <c r="F57" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="G57" s="42"/>
-      <c r="H57" s="42"/>
+      <c r="G57" s="61"/>
+      <c r="H57" s="61"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B58" s="39" t="s">
@@ -9789,16 +9792,16 @@
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C66" s="42" t="s">
+      <c r="C66" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="D66" s="42"/>
-      <c r="E66" s="42"/>
-      <c r="F66" s="43" t="s">
+      <c r="D66" s="61"/>
+      <c r="E66" s="61"/>
+      <c r="F66" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="G66" s="44"/>
-      <c r="H66" s="45"/>
+      <c r="G66" s="63"/>
+      <c r="H66" s="64"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B67" s="39" t="s">
@@ -10042,16 +10045,16 @@
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C76" s="42" t="s">
+      <c r="C76" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="D76" s="42"/>
-      <c r="E76" s="42"/>
-      <c r="F76" s="43" t="s">
+      <c r="D76" s="61"/>
+      <c r="E76" s="61"/>
+      <c r="F76" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="G76" s="44"/>
-      <c r="H76" s="45"/>
+      <c r="G76" s="63"/>
+      <c r="H76" s="64"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B77" s="39" t="s">
@@ -10296,33 +10299,13 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="N3:N6"/>
-    <mergeCell ref="N7:N10"/>
-    <mergeCell ref="N11:N14"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="M31:N31"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="S20:T20"/>
-    <mergeCell ref="S21:T21"/>
-    <mergeCell ref="S27:T27"/>
-    <mergeCell ref="O21:O23"/>
-    <mergeCell ref="O24:O26"/>
-    <mergeCell ref="O27:O29"/>
+    <mergeCell ref="C76:E76"/>
+    <mergeCell ref="F76:H76"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="F57:H57"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="F66:H66"/>
     <mergeCell ref="A34:C34"/>
     <mergeCell ref="A42:C42"/>
     <mergeCell ref="C19:D19"/>
@@ -10339,13 +10322,33 @@
     <mergeCell ref="U24:U26"/>
     <mergeCell ref="S25:T25"/>
     <mergeCell ref="S26:T26"/>
-    <mergeCell ref="C76:E76"/>
-    <mergeCell ref="F76:H76"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="F57:H57"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="S20:T20"/>
+    <mergeCell ref="S21:T21"/>
+    <mergeCell ref="S27:T27"/>
+    <mergeCell ref="O21:O23"/>
+    <mergeCell ref="O24:O26"/>
+    <mergeCell ref="O27:O29"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="N3:N6"/>
+    <mergeCell ref="N7:N10"/>
+    <mergeCell ref="N11:N14"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="C9:C11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -10357,8 +10360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{381D0484-332C-4CA3-8A41-5DD9C3E4C352}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10372,8 +10375,8 @@
       <c r="A1" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="41">
-        <v>119</v>
+      <c r="B1" s="41" t="s">
+        <v>57</v>
       </c>
       <c r="C1" s="41" t="s">
         <v>56</v>
@@ -10902,7 +10905,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="A1:XFD1048576"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10916,8 +10919,8 @@
       <c r="A1" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="41">
-        <v>119</v>
+      <c r="B1" s="41" t="s">
+        <v>57</v>
       </c>
       <c r="C1" s="41" t="s">
         <v>56</v>
@@ -11446,7 +11449,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="A1:XFD1048576"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11460,8 +11463,8 @@
       <c r="A1" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="41">
-        <v>119</v>
+      <c r="B1" s="41" t="s">
+        <v>57</v>
       </c>
       <c r="C1" s="41" t="s">
         <v>56</v>
@@ -11989,8 +11992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0656B60B-719F-400A-BE92-F6DEDEF6288E}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F23" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12004,8 +12007,8 @@
       <c r="A1" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="41">
-        <v>119</v>
+      <c r="B1" s="41" t="s">
+        <v>57</v>
       </c>
       <c r="C1" s="41" t="s">
         <v>56</v>
@@ -12534,7 +12537,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="A1:XFD1048576"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12548,8 +12551,8 @@
       <c r="A1" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="41">
-        <v>119</v>
+      <c r="B1" s="41" t="s">
+        <v>57</v>
       </c>
       <c r="C1" s="41" t="s">
         <v>56</v>
@@ -13077,8 +13080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA00417E-F762-421F-8BAB-E2C762F84677}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13092,8 +13095,8 @@
       <c r="A1" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="41">
-        <v>119</v>
+      <c r="B1" s="41" t="s">
+        <v>57</v>
       </c>
       <c r="C1" s="41" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
add New Cl max and Change Delta CD
</commit_message>
<xml_diff>
--- a/Matching Diagram/Climb.xlsx
+++ b/Matching Diagram/Climb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\Airplane-Design-II\Matching Diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54B6086-E378-4EEC-A08A-2905F150493E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508B870A-77E0-49A5-94AF-199045AE2C2E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{90B7881E-F26A-4004-B09D-A06CC16A62D7}"/>
   </bookViews>
@@ -908,22 +908,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.15737786393876987</c:v>
+                  <c:v>0.19724816049148808</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.15737786393876987</c:v>
+                  <c:v>0.19724816049148808</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.15737786393876987</c:v>
+                  <c:v>0.19724816049148808</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.15737786393876987</c:v>
+                  <c:v>0.19724816049148808</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.15737786393876987</c:v>
+                  <c:v>0.19724816049148808</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.15737786393876987</c:v>
+                  <c:v>0.19724816049148808</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -999,22 +999,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.51234035579766046</c:v>
+                  <c:v>0.58698331354590616</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.51234035579766046</c:v>
+                  <c:v>0.58698331354590616</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.51234035579766046</c:v>
+                  <c:v>0.58698331354590616</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.51234035579766046</c:v>
+                  <c:v>0.58698331354590616</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.51234035579766046</c:v>
+                  <c:v>0.58698331354590616</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.51234035579766046</c:v>
+                  <c:v>0.58698331354590616</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1090,22 +1090,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.16553512410746357</c:v>
+                  <c:v>0.12920424255012972</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.16553512410746357</c:v>
+                  <c:v>0.12920424255012972</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.16553512410746357</c:v>
+                  <c:v>0.12920424255012972</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.16553512410746357</c:v>
+                  <c:v>0.12920424255012972</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.16553512410746357</c:v>
+                  <c:v>0.12920424255012972</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.16553512410746357</c:v>
+                  <c:v>0.12920424255012972</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1522,22 +1522,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.18396266417717397</c:v>
+                  <c:v>0.19709699600961719</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.18396266417717397</c:v>
+                  <c:v>0.19709699600961719</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.18396266417717397</c:v>
+                  <c:v>0.19709699600961719</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.18396266417717397</c:v>
+                  <c:v>0.19709699600961719</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.18396266417717397</c:v>
+                  <c:v>0.19709699600961719</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.18396266417717397</c:v>
+                  <c:v>0.19709699600961719</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1704,22 +1704,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.14827258585743244</c:v>
+                  <c:v>0.13584532727168921</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.14827258585743244</c:v>
+                  <c:v>0.13584532727168921</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.14827258585743244</c:v>
+                  <c:v>0.13584532727168921</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.14827258585743244</c:v>
+                  <c:v>0.13584532727168921</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.14827258585743244</c:v>
+                  <c:v>0.13584532727168921</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.14827258585743244</c:v>
+                  <c:v>0.13584532727168921</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2136,22 +2136,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.17820532252267487</c:v>
+                  <c:v>0.19513581000359276</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.17820532252267487</c:v>
+                  <c:v>0.19513581000359276</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.17820532252267487</c:v>
+                  <c:v>0.19513581000359276</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.17820532252267487</c:v>
+                  <c:v>0.19513581000359276</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.17820532252267487</c:v>
+                  <c:v>0.19513581000359276</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.17820532252267487</c:v>
+                  <c:v>0.19513581000359276</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2227,22 +2227,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.51902198419218926</c:v>
+                  <c:v>0.56843653876385147</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.51902198419218926</c:v>
+                  <c:v>0.56843653876385147</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.51902198419218926</c:v>
+                  <c:v>0.56843653876385147</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.51902198419218926</c:v>
+                  <c:v>0.56843653876385147</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.51902198419218926</c:v>
+                  <c:v>0.56843653876385147</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.51902198419218926</c:v>
+                  <c:v>0.56843653876385147</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2318,22 +2318,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.17651342637510331</c:v>
+                  <c:v>0.14593872489654086</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.17651342637510331</c:v>
+                  <c:v>0.14593872489654086</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.17651342637510331</c:v>
+                  <c:v>0.14593872489654086</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.17651342637510331</c:v>
+                  <c:v>0.14593872489654086</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.17651342637510331</c:v>
+                  <c:v>0.14593872489654086</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.17651342637510331</c:v>
+                  <c:v>0.14593872489654086</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2750,22 +2750,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.15848949866099207</c:v>
+                  <c:v>0.19798925030630293</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.15848949866099207</c:v>
+                  <c:v>0.19798925030630293</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.15848949866099207</c:v>
+                  <c:v>0.19798925030630293</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.15848949866099207</c:v>
+                  <c:v>0.19798925030630293</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.15848949866099207</c:v>
+                  <c:v>0.19798925030630293</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.15848949866099207</c:v>
+                  <c:v>0.19798925030630293</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2841,22 +2841,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.51234035579766046</c:v>
+                  <c:v>0.58698331354590616</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.51234035579766046</c:v>
+                  <c:v>0.58698331354590616</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.51234035579766046</c:v>
+                  <c:v>0.58698331354590616</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.51234035579766046</c:v>
+                  <c:v>0.58698331354590616</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.51234035579766046</c:v>
+                  <c:v>0.58698331354590616</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.51234035579766046</c:v>
+                  <c:v>0.58698331354590616</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2932,22 +2932,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.16998166299635245</c:v>
+                  <c:v>0.13216860180938897</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.16998166299635245</c:v>
+                  <c:v>0.13216860180938897</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.16998166299635245</c:v>
+                  <c:v>0.13216860180938897</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.16998166299635245</c:v>
+                  <c:v>0.13216860180938897</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.16998166299635245</c:v>
+                  <c:v>0.13216860180938897</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.16998166299635245</c:v>
+                  <c:v>0.13216860180938897</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3364,22 +3364,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.18470375399198879</c:v>
+                  <c:v>0.19776397684295052</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.18470375399198879</c:v>
+                  <c:v>0.19776397684295052</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.18470375399198879</c:v>
+                  <c:v>0.19776397684295052</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.18470375399198879</c:v>
+                  <c:v>0.19776397684295052</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.18470375399198879</c:v>
+                  <c:v>0.19776397684295052</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.18470375399198879</c:v>
+                  <c:v>0.19776397684295052</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3546,22 +3546,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.15123694511669172</c:v>
+                  <c:v>0.13851325060502259</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.15123694511669172</c:v>
+                  <c:v>0.13851325060502259</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.15123694511669172</c:v>
+                  <c:v>0.13851325060502259</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.15123694511669172</c:v>
+                  <c:v>0.13851325060502259</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.15123694511669172</c:v>
+                  <c:v>0.13851325060502259</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.15123694511669172</c:v>
+                  <c:v>0.13851325060502259</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3978,22 +3978,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.17891994484410348</c:v>
+                  <c:v>0.19576110453484274</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.17891994484410348</c:v>
+                  <c:v>0.19576110453484274</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.17891994484410348</c:v>
+                  <c:v>0.19576110453484274</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.17891994484410348</c:v>
+                  <c:v>0.19576110453484274</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.17891994484410348</c:v>
+                  <c:v>0.19576110453484274</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.17891994484410348</c:v>
+                  <c:v>0.19576110453484274</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4069,22 +4069,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.52235058419218916</c:v>
+                  <c:v>0.57136570676385146</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.52235058419218916</c:v>
+                  <c:v>0.57136570676385146</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.52235058419218916</c:v>
+                  <c:v>0.57136570676385146</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.52235058419218916</c:v>
+                  <c:v>0.57136570676385146</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.52235058419218916</c:v>
+                  <c:v>0.57136570676385146</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.52235058419218916</c:v>
+                  <c:v>0.57136570676385146</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4160,22 +4160,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.17937191566081756</c:v>
+                  <c:v>0.14843990302154086</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.17937191566081756</c:v>
+                  <c:v>0.14843990302154086</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.17937191566081756</c:v>
+                  <c:v>0.14843990302154086</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.17937191566081756</c:v>
+                  <c:v>0.14843990302154086</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.17937191566081756</c:v>
+                  <c:v>0.14843990302154086</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.17937191566081756</c:v>
+                  <c:v>0.14843990302154086</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8445,8 +8445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AC84584-1541-4318-9FBD-F89612D9C3B7}">
   <dimension ref="A1:W84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8539,7 +8539,7 @@
       </c>
       <c r="N4" s="42"/>
       <c r="O4" s="11">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
@@ -8555,7 +8555,7 @@
       </c>
       <c r="N5" s="42"/>
       <c r="O5" s="11">
-        <v>7.4999999999999997E-2</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="6" spans="2:15" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -8585,7 +8585,7 @@
       </c>
       <c r="N6" s="42"/>
       <c r="O6" s="11">
-        <v>2.5000000000000001E-2</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
@@ -8600,13 +8600,13 @@
         <v>25</v>
       </c>
       <c r="H7" s="18">
-        <v>1.8</v>
+        <v>2.7</v>
       </c>
       <c r="I7" s="18">
-        <v>1.6</v>
+        <v>1.9</v>
       </c>
       <c r="J7" s="18">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="M7" s="10" t="s">
         <v>5</v>
@@ -8630,7 +8630,7 @@
         <v>26</v>
       </c>
       <c r="H8" s="19">
-        <v>2.7</v>
+        <v>3</v>
       </c>
       <c r="I8" s="19">
         <v>2.2000000000000002</v>
@@ -8660,13 +8660,13 @@
         <v>27</v>
       </c>
       <c r="H9" s="20">
-        <v>2.8</v>
+        <v>3.2</v>
       </c>
       <c r="I9" s="20">
-        <v>2.2000000000000002</v>
+        <v>2.5</v>
       </c>
       <c r="J9" s="20">
-        <v>1.8</v>
+        <v>1.7</v>
       </c>
       <c r="M9" s="10" t="s">
         <v>15</v>
@@ -8851,11 +8851,11 @@
       </c>
       <c r="P21" s="24">
         <f>$G$3+$G$21*$G$27^2+$O$6</f>
-        <v>0.17064662010569814</v>
+        <v>0.33736864523782073</v>
       </c>
       <c r="Q21" s="11">
         <f>G27/P21</f>
-        <v>7.9758895915499473</v>
+        <v>6.0515045796924918</v>
       </c>
       <c r="S21" s="48" t="s">
         <v>16</v>
@@ -8866,11 +8866,11 @@
       </c>
       <c r="V21" s="24">
         <f>$G$4+$G$21*$G$27^2+$O$6</f>
-        <v>0.17215962010569813</v>
+        <v>0.33888164523782083</v>
       </c>
       <c r="W21" s="26">
         <f>G27/V21</f>
-        <v>7.905794635807097</v>
+        <v>6.0244865143657318</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
@@ -8903,11 +8903,11 @@
       <c r="O22" s="42"/>
       <c r="P22" s="24">
         <f>$G$3+$G$21*$G$27^2+$O$5</f>
-        <v>0.22064662010569813</v>
+        <v>0.38736864523782077</v>
       </c>
       <c r="Q22" s="11">
         <f>G27/P22</f>
-        <v>6.1684996601453355</v>
+        <v>5.2704005004016601</v>
       </c>
       <c r="S22" s="48" t="s">
         <v>19</v>
@@ -8916,11 +8916,11 @@
       <c r="U22" s="42"/>
       <c r="V22" s="24">
         <f>$G$4+$G$21*$G$27^2+$O$5</f>
-        <v>0.22215962010569812</v>
+        <v>0.38888164523782082</v>
       </c>
       <c r="W22" s="26">
         <f>G27/V22</f>
-        <v>6.1264895955739274</v>
+        <v>5.2498952488559576</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
@@ -8952,11 +8952,11 @@
       <c r="O23" s="42"/>
       <c r="P23" s="24">
         <f>$G$3+$J$21*$J$27^2+$O$4</f>
-        <v>0.15350094406534229</v>
+        <v>0.21158435862339284</v>
       </c>
       <c r="Q23" s="11">
         <f>J27/P23</f>
-        <v>8.6143707951652342</v>
+        <v>7.421380030644146</v>
       </c>
       <c r="S23" s="48" t="s">
         <v>17</v>
@@ -8965,11 +8965,11 @@
       <c r="U23" s="42"/>
       <c r="V23" s="24">
         <f>$G$3+$J$21*$J$27^2+$O$4</f>
-        <v>0.15350094406534229</v>
+        <v>0.21158435862339284</v>
       </c>
       <c r="W23" s="26">
         <f>J27/V23</f>
-        <v>8.6143707951652342</v>
+        <v>7.421380030644146</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
@@ -8982,11 +8982,11 @@
       </c>
       <c r="P24" s="24">
         <f>$G$3+$G$22*$G$28^2+$O$10</f>
-        <v>0.3102451366944195</v>
+        <v>0.37451114406718461</v>
       </c>
       <c r="Q24" s="11">
         <f>G28/P24</f>
-        <v>6.5805637550161364</v>
+        <v>6.0570453985834378</v>
       </c>
       <c r="S24" s="48" t="s">
         <v>16</v>
@@ -8997,11 +8997,11 @@
       </c>
       <c r="V24" s="24">
         <f>$G$4+$G$22*$G$28^2+$O$10</f>
-        <v>0.31175813669441954</v>
+        <v>0.37602414406718465</v>
       </c>
       <c r="W24" s="26">
         <f>G28/V24</f>
-        <v>6.5486274820228871</v>
+        <v>6.0326737994916</v>
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
@@ -9024,11 +9024,11 @@
       <c r="O25" s="42"/>
       <c r="P25" s="24">
         <f>$G$3+$G$22*$G$28^2+$O$9</f>
-        <v>0.35524513669441948</v>
+        <v>0.41951114406718459</v>
       </c>
       <c r="Q25" s="11">
         <f>G28/P25</f>
-        <v>5.7469833948986322</v>
+        <v>5.4073200056088879</v>
       </c>
       <c r="S25" s="48" t="s">
         <v>19</v>
@@ -9037,11 +9037,11 @@
       <c r="U25" s="42"/>
       <c r="V25" s="24">
         <f>$G$4+$G$22*$G$28^2+$O$9</f>
-        <v>0.35675813669441953</v>
+        <v>0.42102414406718464</v>
       </c>
       <c r="W25" s="26">
         <f>G28/V25</f>
-        <v>5.7226106196704398</v>
+        <v>5.387888162367183</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
@@ -9096,21 +9096,21 @@
       </c>
       <c r="D27" s="20">
         <f>J7/1.3^2</f>
-        <v>0.71005917159763299</v>
+        <v>0.76923076923076916</v>
       </c>
       <c r="F27" s="17" t="s">
         <v>25</v>
       </c>
       <c r="G27" s="20">
         <f>H7/$B$31^2</f>
-        <v>1.3610586011342158</v>
+        <v>2.0415879017013236</v>
       </c>
       <c r="I27" s="17" t="s">
         <v>25</v>
       </c>
       <c r="J27" s="23">
         <f>I7/$B$32^2</f>
-        <v>1.3223140495867767</v>
+        <v>1.5702479338842972</v>
       </c>
       <c r="M27" s="48" t="s">
         <v>16</v>
@@ -9121,11 +9121,11 @@
       </c>
       <c r="P27" s="24">
         <f>$G$3+$G$23*$G$29^2+$O$14</f>
-        <v>0.30954624050169355</v>
+        <v>0.3947331508593549</v>
       </c>
       <c r="Q27" s="11">
         <f>G29/P27</f>
-        <v>6.8396962760703239</v>
+        <v>6.1298619841834663</v>
       </c>
       <c r="S27" s="48" t="s">
         <v>16</v>
@@ -9136,11 +9136,11 @@
       </c>
       <c r="V27" s="24">
         <f>$G$4+$G$23*$G$29^2+$O$14</f>
-        <v>0.31105924050169359</v>
+        <v>0.39624615085935494</v>
       </c>
       <c r="W27" s="26">
         <f>G29/V27</f>
-        <v>6.806427820682198</v>
+        <v>6.1064561260774486</v>
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
@@ -9156,7 +9156,7 @@
       </c>
       <c r="G28" s="20">
         <f>H8/$B$31^2</f>
-        <v>2.0415879017013236</v>
+        <v>2.2684310018903595</v>
       </c>
       <c r="I28" s="17" t="s">
         <v>26</v>
@@ -9172,11 +9172,11 @@
       <c r="O28" s="42"/>
       <c r="P28" s="24">
         <f>$G$3+$G$23*$G$29^2+$O$13</f>
-        <v>0.34954624050169353</v>
+        <v>0.43473315085935488</v>
       </c>
       <c r="Q28" s="11">
         <f>G29/P28</f>
-        <v>6.0570019731645335</v>
+        <v>5.5658505236296705</v>
       </c>
       <c r="S28" s="48" t="s">
         <v>19</v>
@@ -9185,11 +9185,11 @@
       <c r="U28" s="42"/>
       <c r="V28" s="24">
         <f>$G$4+$G$23*$G$29^2+$O$13</f>
-        <v>0.35105924050169357</v>
+        <v>0.43624615085935492</v>
       </c>
       <c r="W28" s="26">
         <f>G29/V28</f>
-        <v>6.0308974217722904</v>
+        <v>5.5465468992294022</v>
       </c>
     </row>
     <row r="29" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9198,21 +9198,21 @@
       </c>
       <c r="D29" s="20">
         <f t="shared" si="0"/>
-        <v>1.0650887573964496</v>
+        <v>1.0059171597633134</v>
       </c>
       <c r="F29" s="17" t="s">
         <v>27</v>
       </c>
       <c r="G29" s="20">
         <f>H9/$B$31^2</f>
-        <v>2.1172022684310021</v>
+        <v>2.4196597353497169</v>
       </c>
       <c r="I29" s="17" t="s">
         <v>27</v>
       </c>
       <c r="J29" s="23">
         <f>I9/$B$32^2</f>
-        <v>1.8181818181818181</v>
+        <v>2.0661157024793386</v>
       </c>
       <c r="M29" s="50" t="s">
         <v>17</v>
@@ -9221,11 +9221,11 @@
       <c r="O29" s="43"/>
       <c r="P29" s="27">
         <f>$G$3+$J$23*$J$29^2+$O$12</f>
-        <v>0.21410090190554057</v>
+        <v>0.26882052622099761</v>
       </c>
       <c r="Q29" s="13">
         <f>J29/P29</f>
-        <v>8.4921726251484166</v>
+        <v>7.685855434940942</v>
       </c>
       <c r="S29" s="50" t="s">
         <v>17</v>
@@ -9234,11 +9234,11 @@
       <c r="U29" s="43"/>
       <c r="V29" s="27">
         <f>$G$4+$J$23*$J$29^2+$O$12</f>
-        <v>0.21561390190554056</v>
+        <v>0.2703335262209976</v>
       </c>
       <c r="W29" s="26">
         <f>J29/V29</f>
-        <v>8.4325815826956987</v>
+        <v>7.6428393154250855</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.25">
@@ -9291,19 +9291,19 @@
       </c>
       <c r="P32" s="37">
         <f>$G$3+D21*D27^2</f>
-        <v>4.8159399507265499E-2</v>
+        <v>5.3695927199499102E-2</v>
       </c>
       <c r="Q32" s="37">
         <f>G27/P32</f>
-        <v>28.261535963065356</v>
+        <v>38.021280349925092</v>
       </c>
       <c r="R32" s="37">
         <f>$G$4+D21*D27^2</f>
-        <v>4.9672399507265499E-2</v>
+        <v>5.5208927199499103E-2</v>
       </c>
       <c r="S32" s="37">
         <f>G27/R32</f>
-        <v>27.400701690183823</v>
+        <v>36.979307609510052</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
@@ -9322,7 +9322,7 @@
       </c>
       <c r="Q33" s="37">
         <f t="shared" ref="Q33:Q34" si="2">G28/P33</f>
-        <v>32.187308024545864</v>
+        <v>35.763675582828732</v>
       </c>
       <c r="R33" s="37">
         <f t="shared" ref="R33:R34" si="3">$G$4+D22*D28^2</f>
@@ -9330,7 +9330,7 @@
       </c>
       <c r="S33" s="37">
         <f t="shared" ref="S33:S34" si="4">G28/R33</f>
-        <v>31.437409915268823</v>
+        <v>34.9304554614098</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
@@ -9345,19 +9345,19 @@
       </c>
       <c r="P34" s="37">
         <f t="shared" si="1"/>
-        <v>8.0725443071888336E-2</v>
+        <v>7.3762555703011504E-2</v>
       </c>
       <c r="Q34" s="37">
         <f t="shared" si="2"/>
-        <v>26.227199106799233</v>
+        <v>32.803360896169835</v>
       </c>
       <c r="R34" s="37">
         <f t="shared" si="3"/>
-        <v>8.2238443071888323E-2</v>
+        <v>7.5275555703011504E-2</v>
       </c>
       <c r="S34" s="37">
         <f t="shared" si="4"/>
-        <v>25.74467839305105</v>
+        <v>32.144030193495006</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
@@ -9386,11 +9386,11 @@
       </c>
       <c r="C38" s="24">
         <f>1/Q21+$C$35</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="D38" s="24">
         <f>1/W21+C35</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
@@ -9399,11 +9399,11 @@
       </c>
       <c r="C39" s="24">
         <f>1/Q24+C35</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="D39" s="24">
         <f>1/W24+C35</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
@@ -9412,11 +9412,11 @@
       </c>
       <c r="C40" s="24">
         <f>1/Q27+C35</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="D40" s="24">
         <f>1/W27+C35</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
@@ -9456,11 +9456,11 @@
       </c>
       <c r="C46" s="26">
         <f>($B$30/($B$30-1))*$Q$23^-1+C43</f>
-        <v>0.25617017789883023</v>
+        <v>0.29349165677295308</v>
       </c>
       <c r="D46" s="26">
         <f>($B$30/($B$30-1))*$W$23^-1+C43</f>
-        <v>0.25617017789883023</v>
+        <v>0.29349165677295308</v>
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
@@ -9482,11 +9482,11 @@
       </c>
       <c r="C48" s="26">
         <f>($B$30/($B$30-1))*$Q$29^-1+C43</f>
-        <v>0.25951099209609463</v>
+        <v>0.28421826938192574</v>
       </c>
       <c r="D48" s="26">
         <f>($B$30/($B$30-1))*$W$29^-1+C43</f>
-        <v>0.26117529209609458</v>
+        <v>0.28568285338192573</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -9526,11 +9526,11 @@
       </c>
       <c r="C54" s="26">
         <f>($B$30/($B$30-1))*Q32^-1+$C$51</f>
-        <v>8.2767562053731786E-2</v>
+        <v>6.4602121275064858E-2</v>
       </c>
       <c r="D54" s="26">
         <f>($B$30/($B$30-1))*S32^-1+$C$51</f>
-        <v>8.4990831498176225E-2</v>
+        <v>6.6084300904694485E-2</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -9539,11 +9539,11 @@
       </c>
       <c r="C55" s="26">
         <f t="shared" ref="C55:C56" si="5">($B$30/($B$30-1))*Q33^-1+$C$51</f>
-        <v>7.4136292928716221E-2</v>
+        <v>6.7922663635844607E-2</v>
       </c>
       <c r="D55" s="26">
         <f t="shared" ref="D55:D56" si="6">($B$30/($B$30-1))*S33^-1+$C$51</f>
-        <v>7.5618472558345862E-2</v>
+        <v>6.9256625302511296E-2</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -9552,11 +9552,11 @@
       </c>
       <c r="C56" s="26">
         <f t="shared" si="5"/>
-        <v>8.8256713187551655E-2</v>
+        <v>7.2969362448270431E-2</v>
       </c>
       <c r="D56" s="26">
         <f t="shared" si="6"/>
-        <v>8.968595783040878E-2</v>
+        <v>7.4219951510770432E-2</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -9623,27 +9623,27 @@
       </c>
       <c r="C60" s="21">
         <f>C$38</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="D60" s="21">
         <f>C$39</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="E60" s="21">
         <f>C$40</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="F60" s="21">
         <f>D$38</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="G60" s="21">
         <f>D$39</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="H60" s="21">
         <f>D$40</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -9652,27 +9652,27 @@
       </c>
       <c r="C61" s="21">
         <f t="shared" ref="C61:C65" si="7">C$38</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="D61" s="21">
         <f t="shared" ref="D61:D65" si="8">C$39</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="E61" s="21">
         <f t="shared" ref="E61:E65" si="9">C$40</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="F61" s="21">
         <f t="shared" ref="F61:F65" si="10">D$38</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="G61" s="21">
         <f t="shared" ref="G61:G65" si="11">D$39</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="H61" s="21">
         <f t="shared" ref="H61:H65" si="12">D$40</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -9681,27 +9681,27 @@
       </c>
       <c r="C62" s="21">
         <f t="shared" si="7"/>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="D62" s="21">
         <f t="shared" si="8"/>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="E62" s="21">
         <f t="shared" si="9"/>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="F62" s="21">
         <f t="shared" si="10"/>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="G62" s="21">
         <f t="shared" si="11"/>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="H62" s="21">
         <f t="shared" si="12"/>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -9710,27 +9710,27 @@
       </c>
       <c r="C63" s="21">
         <f t="shared" si="7"/>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="D63" s="21">
         <f t="shared" si="8"/>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="E63" s="21">
         <f t="shared" si="9"/>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="F63" s="21">
         <f t="shared" si="10"/>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="G63" s="21">
         <f t="shared" si="11"/>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="H63" s="21">
         <f t="shared" si="12"/>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -9739,27 +9739,27 @@
       </c>
       <c r="C64" s="21">
         <f t="shared" si="7"/>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="D64" s="21">
         <f t="shared" si="8"/>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="E64" s="21">
         <f t="shared" si="9"/>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="F64" s="21">
         <f t="shared" si="10"/>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="G64" s="21">
         <f t="shared" si="11"/>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="H64" s="21">
         <f t="shared" si="12"/>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -9768,27 +9768,27 @@
       </c>
       <c r="C65" s="21">
         <f t="shared" si="7"/>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="D65" s="21">
         <f t="shared" si="8"/>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="E65" s="21">
         <f t="shared" si="9"/>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="F65" s="21">
         <f t="shared" si="10"/>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="G65" s="21">
         <f t="shared" si="11"/>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="H65" s="21">
         <f t="shared" si="12"/>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -9861,7 +9861,7 @@
       </c>
       <c r="C69" s="21">
         <f>C$46*A69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
       <c r="D69" s="21">
         <f>C$47*A69</f>
@@ -9869,11 +9869,11 @@
       </c>
       <c r="E69" s="21">
         <f>C$48*A69</f>
-        <v>0.51902198419218926</v>
+        <v>0.56843653876385147</v>
       </c>
       <c r="F69" s="21">
         <f>D$46*A69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
       <c r="G69" s="21">
         <f>D$47*A69</f>
@@ -9881,7 +9881,7 @@
       </c>
       <c r="H69" s="21">
         <f>D$48*A69</f>
-        <v>0.52235058419218916</v>
+        <v>0.57136570676385146</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -9893,7 +9893,7 @@
       </c>
       <c r="C70" s="40">
         <f t="shared" ref="C70:C74" si="13">C$46*A70</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
       <c r="D70" s="40">
         <f t="shared" ref="D70:D74" si="14">C$47*A70</f>
@@ -9901,11 +9901,11 @@
       </c>
       <c r="E70" s="40">
         <f t="shared" ref="E70:E74" si="15">C$48*A70</f>
-        <v>0.51902198419218926</v>
+        <v>0.56843653876385147</v>
       </c>
       <c r="F70" s="40">
         <f t="shared" ref="F70:F74" si="16">D$46*A70</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
       <c r="G70" s="40">
         <f t="shared" ref="G70:G74" si="17">D$47*A70</f>
@@ -9913,7 +9913,7 @@
       </c>
       <c r="H70" s="40">
         <f t="shared" ref="H70:H74" si="18">D$48*A70</f>
-        <v>0.52235058419218916</v>
+        <v>0.57136570676385146</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -9925,7 +9925,7 @@
       </c>
       <c r="C71" s="40">
         <f t="shared" si="13"/>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
       <c r="D71" s="40">
         <f t="shared" si="14"/>
@@ -9933,11 +9933,11 @@
       </c>
       <c r="E71" s="40">
         <f t="shared" si="15"/>
-        <v>0.51902198419218926</v>
+        <v>0.56843653876385147</v>
       </c>
       <c r="F71" s="40">
         <f t="shared" si="16"/>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
       <c r="G71" s="40">
         <f t="shared" si="17"/>
@@ -9945,7 +9945,7 @@
       </c>
       <c r="H71" s="40">
         <f t="shared" si="18"/>
-        <v>0.52235058419218916</v>
+        <v>0.57136570676385146</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -9957,7 +9957,7 @@
       </c>
       <c r="C72" s="40">
         <f t="shared" si="13"/>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
       <c r="D72" s="40">
         <f t="shared" si="14"/>
@@ -9965,11 +9965,11 @@
       </c>
       <c r="E72" s="40">
         <f t="shared" si="15"/>
-        <v>0.51902198419218926</v>
+        <v>0.56843653876385147</v>
       </c>
       <c r="F72" s="40">
         <f t="shared" si="16"/>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
       <c r="G72" s="40">
         <f t="shared" si="17"/>
@@ -9977,7 +9977,7 @@
       </c>
       <c r="H72" s="40">
         <f t="shared" si="18"/>
-        <v>0.52235058419218916</v>
+        <v>0.57136570676385146</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -9989,7 +9989,7 @@
       </c>
       <c r="C73" s="40">
         <f t="shared" si="13"/>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
       <c r="D73" s="40">
         <f t="shared" si="14"/>
@@ -9997,11 +9997,11 @@
       </c>
       <c r="E73" s="40">
         <f t="shared" si="15"/>
-        <v>0.51902198419218926</v>
+        <v>0.56843653876385147</v>
       </c>
       <c r="F73" s="40">
         <f t="shared" si="16"/>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
       <c r="G73" s="40">
         <f t="shared" si="17"/>
@@ -10009,7 +10009,7 @@
       </c>
       <c r="H73" s="40">
         <f t="shared" si="18"/>
-        <v>0.52235058419218916</v>
+        <v>0.57136570676385146</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -10021,7 +10021,7 @@
       </c>
       <c r="C74" s="40">
         <f t="shared" si="13"/>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
       <c r="D74" s="40">
         <f t="shared" si="14"/>
@@ -10029,11 +10029,11 @@
       </c>
       <c r="E74" s="40">
         <f t="shared" si="15"/>
-        <v>0.51902198419218926</v>
+        <v>0.56843653876385147</v>
       </c>
       <c r="F74" s="40">
         <f t="shared" si="16"/>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
       <c r="G74" s="40">
         <f t="shared" si="17"/>
@@ -10041,7 +10041,7 @@
       </c>
       <c r="H74" s="40">
         <f t="shared" si="18"/>
-        <v>0.52235058419218916</v>
+        <v>0.57136570676385146</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -10114,27 +10114,27 @@
       </c>
       <c r="C79" s="21">
         <f>C$54*A79</f>
-        <v>0.16553512410746357</v>
+        <v>0.12920424255012972</v>
       </c>
       <c r="D79" s="21">
         <f>C$55*A79</f>
-        <v>0.14827258585743244</v>
+        <v>0.13584532727168921</v>
       </c>
       <c r="E79" s="21">
         <f>C$56*A79</f>
-        <v>0.17651342637510331</v>
+        <v>0.14593872489654086</v>
       </c>
       <c r="F79" s="21">
         <f>D$54*A79</f>
-        <v>0.16998166299635245</v>
+        <v>0.13216860180938897</v>
       </c>
       <c r="G79" s="21">
         <f>D$55*A79</f>
-        <v>0.15123694511669172</v>
+        <v>0.13851325060502259</v>
       </c>
       <c r="H79" s="21">
         <f>D$56*A79</f>
-        <v>0.17937191566081756</v>
+        <v>0.14843990302154086</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -10146,27 +10146,27 @@
       </c>
       <c r="C80" s="40">
         <f t="shared" ref="C80:C84" si="19">C$54*A80</f>
-        <v>0.16553512410746357</v>
+        <v>0.12920424255012972</v>
       </c>
       <c r="D80" s="40">
         <f t="shared" ref="D80:D84" si="20">C$55*A80</f>
-        <v>0.14827258585743244</v>
+        <v>0.13584532727168921</v>
       </c>
       <c r="E80" s="40">
         <f t="shared" ref="E80:E84" si="21">C$56*A80</f>
-        <v>0.17651342637510331</v>
+        <v>0.14593872489654086</v>
       </c>
       <c r="F80" s="40">
         <f t="shared" ref="F80:F84" si="22">D$54*A80</f>
-        <v>0.16998166299635245</v>
+        <v>0.13216860180938897</v>
       </c>
       <c r="G80" s="40">
         <f t="shared" ref="G80:G84" si="23">D$55*A80</f>
-        <v>0.15123694511669172</v>
+        <v>0.13851325060502259</v>
       </c>
       <c r="H80" s="40">
         <f t="shared" ref="H80:H84" si="24">D$56*A80</f>
-        <v>0.17937191566081756</v>
+        <v>0.14843990302154086</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -10178,27 +10178,27 @@
       </c>
       <c r="C81" s="40">
         <f t="shared" si="19"/>
-        <v>0.16553512410746357</v>
+        <v>0.12920424255012972</v>
       </c>
       <c r="D81" s="40">
         <f t="shared" si="20"/>
-        <v>0.14827258585743244</v>
+        <v>0.13584532727168921</v>
       </c>
       <c r="E81" s="40">
         <f t="shared" si="21"/>
-        <v>0.17651342637510331</v>
+        <v>0.14593872489654086</v>
       </c>
       <c r="F81" s="40">
         <f t="shared" si="22"/>
-        <v>0.16998166299635245</v>
+        <v>0.13216860180938897</v>
       </c>
       <c r="G81" s="40">
         <f t="shared" si="23"/>
-        <v>0.15123694511669172</v>
+        <v>0.13851325060502259</v>
       </c>
       <c r="H81" s="40">
         <f t="shared" si="24"/>
-        <v>0.17937191566081756</v>
+        <v>0.14843990302154086</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -10210,27 +10210,27 @@
       </c>
       <c r="C82" s="40">
         <f t="shared" si="19"/>
-        <v>0.16553512410746357</v>
+        <v>0.12920424255012972</v>
       </c>
       <c r="D82" s="40">
         <f t="shared" si="20"/>
-        <v>0.14827258585743244</v>
+        <v>0.13584532727168921</v>
       </c>
       <c r="E82" s="40">
         <f t="shared" si="21"/>
-        <v>0.17651342637510331</v>
+        <v>0.14593872489654086</v>
       </c>
       <c r="F82" s="40">
         <f t="shared" si="22"/>
-        <v>0.16998166299635245</v>
+        <v>0.13216860180938897</v>
       </c>
       <c r="G82" s="40">
         <f t="shared" si="23"/>
-        <v>0.15123694511669172</v>
+        <v>0.13851325060502259</v>
       </c>
       <c r="H82" s="40">
         <f t="shared" si="24"/>
-        <v>0.17937191566081756</v>
+        <v>0.14843990302154086</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -10242,27 +10242,27 @@
       </c>
       <c r="C83" s="40">
         <f t="shared" si="19"/>
-        <v>0.16553512410746357</v>
+        <v>0.12920424255012972</v>
       </c>
       <c r="D83" s="40">
         <f t="shared" si="20"/>
-        <v>0.14827258585743244</v>
+        <v>0.13584532727168921</v>
       </c>
       <c r="E83" s="40">
         <f t="shared" si="21"/>
-        <v>0.17651342637510331</v>
+        <v>0.14593872489654086</v>
       </c>
       <c r="F83" s="40">
         <f t="shared" si="22"/>
-        <v>0.16998166299635245</v>
+        <v>0.13216860180938897</v>
       </c>
       <c r="G83" s="40">
         <f t="shared" si="23"/>
-        <v>0.15123694511669172</v>
+        <v>0.13851325060502259</v>
       </c>
       <c r="H83" s="40">
         <f t="shared" si="24"/>
-        <v>0.17937191566081756</v>
+        <v>0.14843990302154086</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -10274,27 +10274,27 @@
       </c>
       <c r="C84" s="40">
         <f t="shared" si="19"/>
-        <v>0.16553512410746357</v>
+        <v>0.12920424255012972</v>
       </c>
       <c r="D84" s="40">
         <f t="shared" si="20"/>
-        <v>0.14827258585743244</v>
+        <v>0.13584532727168921</v>
       </c>
       <c r="E84" s="40">
         <f t="shared" si="21"/>
-        <v>0.17651342637510331</v>
+        <v>0.14593872489654086</v>
       </c>
       <c r="F84" s="40">
         <f t="shared" si="22"/>
-        <v>0.16998166299635245</v>
+        <v>0.13216860180938897</v>
       </c>
       <c r="G84" s="40">
         <f t="shared" si="23"/>
-        <v>0.15123694511669172</v>
+        <v>0.13851325060502259</v>
       </c>
       <c r="H84" s="40">
         <f t="shared" si="24"/>
-        <v>0.17937191566081756</v>
+        <v>0.14843990302154086</v>
       </c>
     </row>
   </sheetData>
@@ -10391,15 +10391,15 @@
       </c>
       <c r="B2">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="C2">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="D2">
         <f>Sheet1!$C$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -10408,15 +10408,15 @@
       </c>
       <c r="B3">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="C3">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="D3">
         <f>Sheet1!$C$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -10425,15 +10425,15 @@
       </c>
       <c r="B4">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="C4">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="D4">
         <f>Sheet1!$C$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -10442,15 +10442,15 @@
       </c>
       <c r="B5">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="C5">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="D5">
         <f>Sheet1!$C$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -10459,15 +10459,15 @@
       </c>
       <c r="B6">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="C6">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="D6">
         <f>Sheet1!$C$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -10476,15 +10476,15 @@
       </c>
       <c r="B7">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="C7">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="D7">
         <f>Sheet1!$C$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -10493,15 +10493,15 @@
       </c>
       <c r="B8">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="C8">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="D8">
         <f>Sheet1!$C$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -10510,15 +10510,15 @@
       </c>
       <c r="B9">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="C9">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="D9">
         <f>Sheet1!$C$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -10527,15 +10527,15 @@
       </c>
       <c r="B10">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="C10">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="D10">
         <f>Sheet1!$C$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -10544,15 +10544,15 @@
       </c>
       <c r="B11">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="C11">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="D11">
         <f>Sheet1!$C$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -10561,15 +10561,15 @@
       </c>
       <c r="B12">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="C12">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="D12">
         <f>Sheet1!$C$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -10578,15 +10578,15 @@
       </c>
       <c r="B13">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="C13">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="D13">
         <f>Sheet1!$C$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -10595,15 +10595,15 @@
       </c>
       <c r="B14">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="C14">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="D14">
         <f>Sheet1!$C$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -10612,15 +10612,15 @@
       </c>
       <c r="B15">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="C15">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="D15">
         <f>Sheet1!$C$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -10629,15 +10629,15 @@
       </c>
       <c r="B16">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="C16">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="D16">
         <f>Sheet1!$C$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -10646,15 +10646,15 @@
       </c>
       <c r="B17">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="C17">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="D17">
         <f>Sheet1!$C$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -10663,15 +10663,15 @@
       </c>
       <c r="B18">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="C18">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="D18">
         <f>Sheet1!$C$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -10680,15 +10680,15 @@
       </c>
       <c r="B19">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="C19">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="D19">
         <f>Sheet1!$C$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -10697,15 +10697,15 @@
       </c>
       <c r="B20">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="C20">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="D20">
         <f>Sheet1!$C$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -10714,15 +10714,15 @@
       </c>
       <c r="B21">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="C21">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="D21">
         <f>Sheet1!$C$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -10731,15 +10731,15 @@
       </c>
       <c r="B22">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="C22">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="D22">
         <f>Sheet1!$C$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -10748,15 +10748,15 @@
       </c>
       <c r="B23">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="C23">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="D23">
         <f>Sheet1!$C$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -10765,15 +10765,15 @@
       </c>
       <c r="B24">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="C24">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="D24">
         <f>Sheet1!$C$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -10782,15 +10782,15 @@
       </c>
       <c r="B25">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="C25">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="D25">
         <f>Sheet1!$C$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -10799,15 +10799,15 @@
       </c>
       <c r="B26">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="C26">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="D26">
         <f>Sheet1!$C$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -10816,15 +10816,15 @@
       </c>
       <c r="B27">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="C27">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="D27">
         <f>Sheet1!$C$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -10833,15 +10833,15 @@
       </c>
       <c r="B28">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="C28">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="D28">
         <f>Sheet1!$C$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -10850,15 +10850,15 @@
       </c>
       <c r="B29">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="C29">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="D29">
         <f>Sheet1!$C$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -10867,15 +10867,15 @@
       </c>
       <c r="B30">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="C30">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="D30">
         <f>Sheet1!$C$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -10884,15 +10884,15 @@
       </c>
       <c r="B31">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="C31">
         <f>Sheet1!$C$60</f>
-        <v>0.15737786393876987</v>
+        <v>0.19724816049148808</v>
       </c>
       <c r="D31">
         <f>Sheet1!$C$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
   </sheetData>
@@ -10935,11 +10935,11 @@
       </c>
       <c r="B2">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="C2">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="D2">
         <f>Sheet1!$D$69</f>
@@ -10952,11 +10952,11 @@
       </c>
       <c r="B3">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="C3">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="D3">
         <f>Sheet1!$D$69</f>
@@ -10969,11 +10969,11 @@
       </c>
       <c r="B4">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="C4">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="D4">
         <f>Sheet1!$D$69</f>
@@ -10986,11 +10986,11 @@
       </c>
       <c r="B5">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="C5">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="D5">
         <f>Sheet1!$D$69</f>
@@ -11003,11 +11003,11 @@
       </c>
       <c r="B6">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="C6">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="D6">
         <f>Sheet1!$D$69</f>
@@ -11020,11 +11020,11 @@
       </c>
       <c r="B7">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="C7">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="D7">
         <f>Sheet1!$D$69</f>
@@ -11037,11 +11037,11 @@
       </c>
       <c r="B8">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="C8">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="D8">
         <f>Sheet1!$D$69</f>
@@ -11054,11 +11054,11 @@
       </c>
       <c r="B9">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="C9">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="D9">
         <f>Sheet1!$D$69</f>
@@ -11071,11 +11071,11 @@
       </c>
       <c r="B10">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="C10">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="D10">
         <f>Sheet1!$D$69</f>
@@ -11088,11 +11088,11 @@
       </c>
       <c r="B11">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="C11">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="D11">
         <f>Sheet1!$D$69</f>
@@ -11105,11 +11105,11 @@
       </c>
       <c r="B12">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="C12">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="D12">
         <f>Sheet1!$D$69</f>
@@ -11122,11 +11122,11 @@
       </c>
       <c r="B13">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="C13">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="D13">
         <f>Sheet1!$D$69</f>
@@ -11139,11 +11139,11 @@
       </c>
       <c r="B14">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="C14">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="D14">
         <f>Sheet1!$D$69</f>
@@ -11156,11 +11156,11 @@
       </c>
       <c r="B15">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="C15">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="D15">
         <f>Sheet1!$D$69</f>
@@ -11173,11 +11173,11 @@
       </c>
       <c r="B16">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="C16">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="D16">
         <f>Sheet1!$D$69</f>
@@ -11190,11 +11190,11 @@
       </c>
       <c r="B17">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="C17">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="D17">
         <f>Sheet1!$D$69</f>
@@ -11207,11 +11207,11 @@
       </c>
       <c r="B18">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="C18">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="D18">
         <f>Sheet1!$D$69</f>
@@ -11224,11 +11224,11 @@
       </c>
       <c r="B19">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="C19">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="D19">
         <f>Sheet1!$D$69</f>
@@ -11241,11 +11241,11 @@
       </c>
       <c r="B20">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="C20">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="D20">
         <f>Sheet1!$D$69</f>
@@ -11258,11 +11258,11 @@
       </c>
       <c r="B21">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="C21">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="D21">
         <f>Sheet1!$D$69</f>
@@ -11275,11 +11275,11 @@
       </c>
       <c r="B22">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="C22">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="D22">
         <f>Sheet1!$D$69</f>
@@ -11292,11 +11292,11 @@
       </c>
       <c r="B23">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="C23">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="D23">
         <f>Sheet1!$D$69</f>
@@ -11309,11 +11309,11 @@
       </c>
       <c r="B24">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="C24">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="D24">
         <f>Sheet1!$D$69</f>
@@ -11326,11 +11326,11 @@
       </c>
       <c r="B25">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="C25">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="D25">
         <f>Sheet1!$D$69</f>
@@ -11343,11 +11343,11 @@
       </c>
       <c r="B26">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="C26">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="D26">
         <f>Sheet1!$D$69</f>
@@ -11360,11 +11360,11 @@
       </c>
       <c r="B27">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="C27">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="D27">
         <f>Sheet1!$D$69</f>
@@ -11377,11 +11377,11 @@
       </c>
       <c r="B28">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="C28">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="D28">
         <f>Sheet1!$D$69</f>
@@ -11394,11 +11394,11 @@
       </c>
       <c r="B29">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="C29">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="D29">
         <f>Sheet1!$D$69</f>
@@ -11411,11 +11411,11 @@
       </c>
       <c r="B30">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="C30">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="D30">
         <f>Sheet1!$D$69</f>
@@ -11428,11 +11428,11 @@
       </c>
       <c r="B31">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="C31">
         <f>Sheet1!$D$60</f>
-        <v>0.18396266417717397</v>
+        <v>0.19709699600961719</v>
       </c>
       <c r="D31">
         <f>Sheet1!$D$69</f>
@@ -11479,15 +11479,15 @@
       </c>
       <c r="B2">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="C2">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="D2">
         <f>Sheet1!$E$69</f>
-        <v>0.51902198419218926</v>
+        <v>0.56843653876385147</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -11496,15 +11496,15 @@
       </c>
       <c r="B3">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="C3">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="D3">
         <f>Sheet1!$E$69</f>
-        <v>0.51902198419218926</v>
+        <v>0.56843653876385147</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -11513,15 +11513,15 @@
       </c>
       <c r="B4">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="C4">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="D4">
         <f>Sheet1!$E$69</f>
-        <v>0.51902198419218926</v>
+        <v>0.56843653876385147</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -11530,15 +11530,15 @@
       </c>
       <c r="B5">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="C5">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="D5">
         <f>Sheet1!$E$69</f>
-        <v>0.51902198419218926</v>
+        <v>0.56843653876385147</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -11547,15 +11547,15 @@
       </c>
       <c r="B6">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="C6">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="D6">
         <f>Sheet1!$E$69</f>
-        <v>0.51902198419218926</v>
+        <v>0.56843653876385147</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -11564,15 +11564,15 @@
       </c>
       <c r="B7">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="C7">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="D7">
         <f>Sheet1!$E$69</f>
-        <v>0.51902198419218926</v>
+        <v>0.56843653876385147</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -11581,15 +11581,15 @@
       </c>
       <c r="B8">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="C8">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="D8">
         <f>Sheet1!$E$69</f>
-        <v>0.51902198419218926</v>
+        <v>0.56843653876385147</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -11598,15 +11598,15 @@
       </c>
       <c r="B9">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="C9">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="D9">
         <f>Sheet1!$E$69</f>
-        <v>0.51902198419218926</v>
+        <v>0.56843653876385147</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -11615,15 +11615,15 @@
       </c>
       <c r="B10">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="C10">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="D10">
         <f>Sheet1!$E$69</f>
-        <v>0.51902198419218926</v>
+        <v>0.56843653876385147</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -11632,15 +11632,15 @@
       </c>
       <c r="B11">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="C11">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="D11">
         <f>Sheet1!$E$69</f>
-        <v>0.51902198419218926</v>
+        <v>0.56843653876385147</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -11649,15 +11649,15 @@
       </c>
       <c r="B12">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="C12">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="D12">
         <f>Sheet1!$E$69</f>
-        <v>0.51902198419218926</v>
+        <v>0.56843653876385147</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -11666,15 +11666,15 @@
       </c>
       <c r="B13">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="C13">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="D13">
         <f>Sheet1!$E$69</f>
-        <v>0.51902198419218926</v>
+        <v>0.56843653876385147</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -11683,15 +11683,15 @@
       </c>
       <c r="B14">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="C14">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="D14">
         <f>Sheet1!$E$69</f>
-        <v>0.51902198419218926</v>
+        <v>0.56843653876385147</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -11700,15 +11700,15 @@
       </c>
       <c r="B15">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="C15">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="D15">
         <f>Sheet1!$E$69</f>
-        <v>0.51902198419218926</v>
+        <v>0.56843653876385147</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -11717,15 +11717,15 @@
       </c>
       <c r="B16">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="C16">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="D16">
         <f>Sheet1!$E$69</f>
-        <v>0.51902198419218926</v>
+        <v>0.56843653876385147</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -11734,15 +11734,15 @@
       </c>
       <c r="B17">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="C17">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="D17">
         <f>Sheet1!$E$69</f>
-        <v>0.51902198419218926</v>
+        <v>0.56843653876385147</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -11751,15 +11751,15 @@
       </c>
       <c r="B18">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="C18">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="D18">
         <f>Sheet1!$E$69</f>
-        <v>0.51902198419218926</v>
+        <v>0.56843653876385147</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -11768,15 +11768,15 @@
       </c>
       <c r="B19">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="C19">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="D19">
         <f>Sheet1!$E$69</f>
-        <v>0.51902198419218926</v>
+        <v>0.56843653876385147</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -11785,15 +11785,15 @@
       </c>
       <c r="B20">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="C20">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="D20">
         <f>Sheet1!$E$69</f>
-        <v>0.51902198419218926</v>
+        <v>0.56843653876385147</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -11802,15 +11802,15 @@
       </c>
       <c r="B21">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="C21">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="D21">
         <f>Sheet1!$E$69</f>
-        <v>0.51902198419218926</v>
+        <v>0.56843653876385147</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -11819,15 +11819,15 @@
       </c>
       <c r="B22">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="C22">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="D22">
         <f>Sheet1!$E$69</f>
-        <v>0.51902198419218926</v>
+        <v>0.56843653876385147</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -11836,15 +11836,15 @@
       </c>
       <c r="B23">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="C23">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="D23">
         <f>Sheet1!$E$69</f>
-        <v>0.51902198419218926</v>
+        <v>0.56843653876385147</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -11853,15 +11853,15 @@
       </c>
       <c r="B24">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="C24">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="D24">
         <f>Sheet1!$E$69</f>
-        <v>0.51902198419218926</v>
+        <v>0.56843653876385147</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -11870,15 +11870,15 @@
       </c>
       <c r="B25">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="C25">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="D25">
         <f>Sheet1!$E$69</f>
-        <v>0.51902198419218926</v>
+        <v>0.56843653876385147</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -11887,15 +11887,15 @@
       </c>
       <c r="B26">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="C26">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="D26">
         <f>Sheet1!$E$69</f>
-        <v>0.51902198419218926</v>
+        <v>0.56843653876385147</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -11904,15 +11904,15 @@
       </c>
       <c r="B27">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="C27">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="D27">
         <f>Sheet1!$E$69</f>
-        <v>0.51902198419218926</v>
+        <v>0.56843653876385147</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -11921,15 +11921,15 @@
       </c>
       <c r="B28">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="C28">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="D28">
         <f>Sheet1!$E$69</f>
-        <v>0.51902198419218926</v>
+        <v>0.56843653876385147</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -11938,15 +11938,15 @@
       </c>
       <c r="B29">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="C29">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="D29">
         <f>Sheet1!$E$69</f>
-        <v>0.51902198419218926</v>
+        <v>0.56843653876385147</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -11955,15 +11955,15 @@
       </c>
       <c r="B30">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="C30">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="D30">
         <f>Sheet1!$E$69</f>
-        <v>0.51902198419218926</v>
+        <v>0.56843653876385147</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -11972,15 +11972,15 @@
       </c>
       <c r="B31">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="C31">
         <f>Sheet1!$E$60</f>
-        <v>0.17820532252267487</v>
+        <v>0.19513581000359276</v>
       </c>
       <c r="D31">
         <f>Sheet1!$E$69</f>
-        <v>0.51902198419218926</v>
+        <v>0.56843653876385147</v>
       </c>
     </row>
   </sheetData>
@@ -12023,15 +12023,15 @@
       </c>
       <c r="B2">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="C2">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="D2">
         <f>Sheet1!$F$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -12040,15 +12040,15 @@
       </c>
       <c r="B3">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="C3">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="D3">
         <f>Sheet1!$F$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -12057,15 +12057,15 @@
       </c>
       <c r="B4">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="C4">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="D4">
         <f>Sheet1!$F$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -12074,15 +12074,15 @@
       </c>
       <c r="B5">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="C5">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="D5">
         <f>Sheet1!$F$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -12091,15 +12091,15 @@
       </c>
       <c r="B6">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="C6">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="D6">
         <f>Sheet1!$F$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -12108,15 +12108,15 @@
       </c>
       <c r="B7">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="C7">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="D7">
         <f>Sheet1!$F$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -12125,15 +12125,15 @@
       </c>
       <c r="B8">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="C8">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="D8">
         <f>Sheet1!$F$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -12142,15 +12142,15 @@
       </c>
       <c r="B9">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="C9">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="D9">
         <f>Sheet1!$F$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -12159,15 +12159,15 @@
       </c>
       <c r="B10">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="C10">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="D10">
         <f>Sheet1!$F$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -12176,15 +12176,15 @@
       </c>
       <c r="B11">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="C11">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="D11">
         <f>Sheet1!$F$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -12193,15 +12193,15 @@
       </c>
       <c r="B12">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="C12">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="D12">
         <f>Sheet1!$F$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -12210,15 +12210,15 @@
       </c>
       <c r="B13">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="C13">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="D13">
         <f>Sheet1!$F$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -12227,15 +12227,15 @@
       </c>
       <c r="B14">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="C14">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="D14">
         <f>Sheet1!$F$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -12244,15 +12244,15 @@
       </c>
       <c r="B15">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="C15">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="D15">
         <f>Sheet1!$F$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -12261,15 +12261,15 @@
       </c>
       <c r="B16">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="C16">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="D16">
         <f>Sheet1!$F$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -12278,15 +12278,15 @@
       </c>
       <c r="B17">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="C17">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="D17">
         <f>Sheet1!$F$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -12295,15 +12295,15 @@
       </c>
       <c r="B18">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="C18">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="D18">
         <f>Sheet1!$F$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -12312,15 +12312,15 @@
       </c>
       <c r="B19">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="C19">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="D19">
         <f>Sheet1!$F$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -12329,15 +12329,15 @@
       </c>
       <c r="B20">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="C20">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="D20">
         <f>Sheet1!$F$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -12346,15 +12346,15 @@
       </c>
       <c r="B21">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="C21">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="D21">
         <f>Sheet1!$F$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -12363,15 +12363,15 @@
       </c>
       <c r="B22">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="C22">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="D22">
         <f>Sheet1!$F$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -12380,15 +12380,15 @@
       </c>
       <c r="B23">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="C23">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="D23">
         <f>Sheet1!$F$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -12397,15 +12397,15 @@
       </c>
       <c r="B24">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="C24">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="D24">
         <f>Sheet1!$F$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -12414,15 +12414,15 @@
       </c>
       <c r="B25">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="C25">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="D25">
         <f>Sheet1!$F$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -12431,15 +12431,15 @@
       </c>
       <c r="B26">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="C26">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="D26">
         <f>Sheet1!$F$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -12448,15 +12448,15 @@
       </c>
       <c r="B27">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="C27">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="D27">
         <f>Sheet1!$F$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -12465,15 +12465,15 @@
       </c>
       <c r="B28">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="C28">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="D28">
         <f>Sheet1!$F$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -12482,15 +12482,15 @@
       </c>
       <c r="B29">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="C29">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="D29">
         <f>Sheet1!$F$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -12499,15 +12499,15 @@
       </c>
       <c r="B30">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="C30">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="D30">
         <f>Sheet1!$F$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -12516,15 +12516,15 @@
       </c>
       <c r="B31">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="C31">
         <f>Sheet1!$F$60</f>
-        <v>0.15848949866099207</v>
+        <v>0.19798925030630293</v>
       </c>
       <c r="D31">
         <f>Sheet1!$F$69</f>
-        <v>0.51234035579766046</v>
+        <v>0.58698331354590616</v>
       </c>
     </row>
   </sheetData>
@@ -12567,11 +12567,11 @@
       </c>
       <c r="B2">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="C2">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="D2">
         <f>Sheet1!$G$69</f>
@@ -12584,11 +12584,11 @@
       </c>
       <c r="B3">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="C3">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="D3">
         <f>Sheet1!$G$69</f>
@@ -12601,11 +12601,11 @@
       </c>
       <c r="B4">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="C4">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="D4">
         <f>Sheet1!$G$69</f>
@@ -12618,11 +12618,11 @@
       </c>
       <c r="B5">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="C5">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="D5">
         <f>Sheet1!$G$69</f>
@@ -12635,11 +12635,11 @@
       </c>
       <c r="B6">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="C6">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="D6">
         <f>Sheet1!$G$69</f>
@@ -12652,11 +12652,11 @@
       </c>
       <c r="B7">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="C7">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="D7">
         <f>Sheet1!$G$69</f>
@@ -12669,11 +12669,11 @@
       </c>
       <c r="B8">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="C8">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="D8">
         <f>Sheet1!$G$69</f>
@@ -12686,11 +12686,11 @@
       </c>
       <c r="B9">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="C9">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="D9">
         <f>Sheet1!$G$69</f>
@@ -12703,11 +12703,11 @@
       </c>
       <c r="B10">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="C10">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="D10">
         <f>Sheet1!$G$69</f>
@@ -12720,11 +12720,11 @@
       </c>
       <c r="B11">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="C11">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="D11">
         <f>Sheet1!$G$69</f>
@@ -12737,11 +12737,11 @@
       </c>
       <c r="B12">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="C12">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="D12">
         <f>Sheet1!$G$69</f>
@@ -12754,11 +12754,11 @@
       </c>
       <c r="B13">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="C13">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="D13">
         <f>Sheet1!$G$69</f>
@@ -12771,11 +12771,11 @@
       </c>
       <c r="B14">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="C14">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="D14">
         <f>Sheet1!$G$69</f>
@@ -12788,11 +12788,11 @@
       </c>
       <c r="B15">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="C15">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="D15">
         <f>Sheet1!$G$69</f>
@@ -12805,11 +12805,11 @@
       </c>
       <c r="B16">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="C16">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="D16">
         <f>Sheet1!$G$69</f>
@@ -12822,11 +12822,11 @@
       </c>
       <c r="B17">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="C17">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="D17">
         <f>Sheet1!$G$69</f>
@@ -12839,11 +12839,11 @@
       </c>
       <c r="B18">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="C18">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="D18">
         <f>Sheet1!$G$69</f>
@@ -12856,11 +12856,11 @@
       </c>
       <c r="B19">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="C19">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="D19">
         <f>Sheet1!$G$69</f>
@@ -12873,11 +12873,11 @@
       </c>
       <c r="B20">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="C20">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="D20">
         <f>Sheet1!$G$69</f>
@@ -12890,11 +12890,11 @@
       </c>
       <c r="B21">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="C21">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="D21">
         <f>Sheet1!$G$69</f>
@@ -12907,11 +12907,11 @@
       </c>
       <c r="B22">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="C22">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="D22">
         <f>Sheet1!$G$69</f>
@@ -12924,11 +12924,11 @@
       </c>
       <c r="B23">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="C23">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="D23">
         <f>Sheet1!$G$69</f>
@@ -12941,11 +12941,11 @@
       </c>
       <c r="B24">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="C24">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="D24">
         <f>Sheet1!$G$69</f>
@@ -12958,11 +12958,11 @@
       </c>
       <c r="B25">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="C25">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="D25">
         <f>Sheet1!$G$69</f>
@@ -12975,11 +12975,11 @@
       </c>
       <c r="B26">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="C26">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="D26">
         <f>Sheet1!$G$69</f>
@@ -12992,11 +12992,11 @@
       </c>
       <c r="B27">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="C27">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="D27">
         <f>Sheet1!$G$69</f>
@@ -13009,11 +13009,11 @@
       </c>
       <c r="B28">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="C28">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="D28">
         <f>Sheet1!$G$69</f>
@@ -13026,11 +13026,11 @@
       </c>
       <c r="B29">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="C29">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="D29">
         <f>Sheet1!$G$69</f>
@@ -13043,11 +13043,11 @@
       </c>
       <c r="B30">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="C30">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="D30">
         <f>Sheet1!$G$69</f>
@@ -13060,11 +13060,11 @@
       </c>
       <c r="B31">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="C31">
         <f>Sheet1!$G$60</f>
-        <v>0.18470375399198879</v>
+        <v>0.19776397684295052</v>
       </c>
       <c r="D31">
         <f>Sheet1!$G$69</f>
@@ -13111,15 +13111,15 @@
       </c>
       <c r="B2">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="C2">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="D2">
         <f>Sheet1!$H$69</f>
-        <v>0.52235058419218916</v>
+        <v>0.57136570676385146</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -13128,15 +13128,15 @@
       </c>
       <c r="B3">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="C3">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="D3">
         <f>Sheet1!$H$69</f>
-        <v>0.52235058419218916</v>
+        <v>0.57136570676385146</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -13145,15 +13145,15 @@
       </c>
       <c r="B4">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="C4">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="D4">
         <f>Sheet1!$H$69</f>
-        <v>0.52235058419218916</v>
+        <v>0.57136570676385146</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -13162,15 +13162,15 @@
       </c>
       <c r="B5">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="C5">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="D5">
         <f>Sheet1!$H$69</f>
-        <v>0.52235058419218916</v>
+        <v>0.57136570676385146</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -13179,15 +13179,15 @@
       </c>
       <c r="B6">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="C6">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="D6">
         <f>Sheet1!$H$69</f>
-        <v>0.52235058419218916</v>
+        <v>0.57136570676385146</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -13196,15 +13196,15 @@
       </c>
       <c r="B7">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="C7">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="D7">
         <f>Sheet1!$H$69</f>
-        <v>0.52235058419218916</v>
+        <v>0.57136570676385146</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -13213,15 +13213,15 @@
       </c>
       <c r="B8">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="C8">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="D8">
         <f>Sheet1!$H$69</f>
-        <v>0.52235058419218916</v>
+        <v>0.57136570676385146</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -13230,15 +13230,15 @@
       </c>
       <c r="B9">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="C9">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="D9">
         <f>Sheet1!$H$69</f>
-        <v>0.52235058419218916</v>
+        <v>0.57136570676385146</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -13247,15 +13247,15 @@
       </c>
       <c r="B10">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="C10">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="D10">
         <f>Sheet1!$H$69</f>
-        <v>0.52235058419218916</v>
+        <v>0.57136570676385146</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -13264,15 +13264,15 @@
       </c>
       <c r="B11">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="C11">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="D11">
         <f>Sheet1!$H$69</f>
-        <v>0.52235058419218916</v>
+        <v>0.57136570676385146</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -13281,15 +13281,15 @@
       </c>
       <c r="B12">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="C12">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="D12">
         <f>Sheet1!$H$69</f>
-        <v>0.52235058419218916</v>
+        <v>0.57136570676385146</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -13298,15 +13298,15 @@
       </c>
       <c r="B13">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="C13">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="D13">
         <f>Sheet1!$H$69</f>
-        <v>0.52235058419218916</v>
+        <v>0.57136570676385146</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -13315,15 +13315,15 @@
       </c>
       <c r="B14">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="C14">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="D14">
         <f>Sheet1!$H$69</f>
-        <v>0.52235058419218916</v>
+        <v>0.57136570676385146</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -13332,15 +13332,15 @@
       </c>
       <c r="B15">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="C15">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="D15">
         <f>Sheet1!$H$69</f>
-        <v>0.52235058419218916</v>
+        <v>0.57136570676385146</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -13349,15 +13349,15 @@
       </c>
       <c r="B16">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="C16">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="D16">
         <f>Sheet1!$H$69</f>
-        <v>0.52235058419218916</v>
+        <v>0.57136570676385146</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -13366,15 +13366,15 @@
       </c>
       <c r="B17">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="C17">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="D17">
         <f>Sheet1!$H$69</f>
-        <v>0.52235058419218916</v>
+        <v>0.57136570676385146</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -13383,15 +13383,15 @@
       </c>
       <c r="B18">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="C18">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="D18">
         <f>Sheet1!$H$69</f>
-        <v>0.52235058419218916</v>
+        <v>0.57136570676385146</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -13400,15 +13400,15 @@
       </c>
       <c r="B19">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="C19">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="D19">
         <f>Sheet1!$H$69</f>
-        <v>0.52235058419218916</v>
+        <v>0.57136570676385146</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -13417,15 +13417,15 @@
       </c>
       <c r="B20">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="C20">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="D20">
         <f>Sheet1!$H$69</f>
-        <v>0.52235058419218916</v>
+        <v>0.57136570676385146</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -13434,15 +13434,15 @@
       </c>
       <c r="B21">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="C21">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="D21">
         <f>Sheet1!$H$69</f>
-        <v>0.52235058419218916</v>
+        <v>0.57136570676385146</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -13451,15 +13451,15 @@
       </c>
       <c r="B22">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="C22">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="D22">
         <f>Sheet1!$H$69</f>
-        <v>0.52235058419218916</v>
+        <v>0.57136570676385146</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -13468,15 +13468,15 @@
       </c>
       <c r="B23">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="C23">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="D23">
         <f>Sheet1!$H$69</f>
-        <v>0.52235058419218916</v>
+        <v>0.57136570676385146</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -13485,15 +13485,15 @@
       </c>
       <c r="B24">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="C24">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="D24">
         <f>Sheet1!$H$69</f>
-        <v>0.52235058419218916</v>
+        <v>0.57136570676385146</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -13502,15 +13502,15 @@
       </c>
       <c r="B25">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="C25">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="D25">
         <f>Sheet1!$H$69</f>
-        <v>0.52235058419218916</v>
+        <v>0.57136570676385146</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -13519,15 +13519,15 @@
       </c>
       <c r="B26">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="C26">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="D26">
         <f>Sheet1!$H$69</f>
-        <v>0.52235058419218916</v>
+        <v>0.57136570676385146</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -13536,15 +13536,15 @@
       </c>
       <c r="B27">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="C27">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="D27">
         <f>Sheet1!$H$69</f>
-        <v>0.52235058419218916</v>
+        <v>0.57136570676385146</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -13553,15 +13553,15 @@
       </c>
       <c r="B28">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="C28">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="D28">
         <f>Sheet1!$H$69</f>
-        <v>0.52235058419218916</v>
+        <v>0.57136570676385146</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -13570,15 +13570,15 @@
       </c>
       <c r="B29">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="C29">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="D29">
         <f>Sheet1!$H$69</f>
-        <v>0.52235058419218916</v>
+        <v>0.57136570676385146</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -13587,15 +13587,15 @@
       </c>
       <c r="B30">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="C30">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="D30">
         <f>Sheet1!$H$69</f>
-        <v>0.52235058419218916</v>
+        <v>0.57136570676385146</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -13604,15 +13604,15 @@
       </c>
       <c r="B31">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="C31">
         <f>Sheet1!$H$60</f>
-        <v>0.17891994484410348</v>
+        <v>0.19576110453484274</v>
       </c>
       <c r="D31">
         <f>Sheet1!$H$69</f>
-        <v>0.52235058419218916</v>
+        <v>0.57136570676385146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix Climb excel and Turn AR and CD0
</commit_message>
<xml_diff>
--- a/Matching Diagram/Climb.xlsx
+++ b/Matching Diagram/Climb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\Airplane-Design-II\Matching Diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508B870A-77E0-49A5-94AF-199045AE2C2E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66101608-C8C2-4B35-B093-93B398AB34B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{90B7881E-F26A-4004-B09D-A06CC16A62D7}"/>
   </bookViews>
@@ -737,22 +737,28 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -767,21 +773,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -794,17 +785,26 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -8445,8 +8445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AC84584-1541-4318-9FBD-F89612D9C3B7}">
   <dimension ref="A1:W84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E69" sqref="E69"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H81" sqref="H81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8498,7 +8498,7 @@
       <c r="B3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="61" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="11">
@@ -8513,7 +8513,7 @@
       <c r="M3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="42" t="s">
+      <c r="N3" s="48" t="s">
         <v>3</v>
       </c>
       <c r="O3" s="11">
@@ -8524,7 +8524,7 @@
       <c r="B4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="45"/>
+      <c r="C4" s="62"/>
       <c r="D4" s="11">
         <v>0.5</v>
       </c>
@@ -8537,7 +8537,7 @@
       <c r="M4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="N4" s="42"/>
+      <c r="N4" s="48"/>
       <c r="O4" s="11">
         <v>0.03</v>
       </c>
@@ -8546,14 +8546,14 @@
       <c r="B5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="46"/>
+      <c r="C5" s="63"/>
       <c r="D5" s="11">
         <v>0.48</v>
       </c>
       <c r="M5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="N5" s="42"/>
+      <c r="N5" s="48"/>
       <c r="O5" s="11">
         <v>0.08</v>
       </c>
@@ -8562,7 +8562,7 @@
       <c r="B6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="44" t="s">
+      <c r="C6" s="61" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="11">
@@ -8583,7 +8583,7 @@
       <c r="M6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="N6" s="42"/>
+      <c r="N6" s="48"/>
       <c r="O6" s="11">
         <v>0.03</v>
       </c>
@@ -8592,7 +8592,7 @@
       <c r="B7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="45"/>
+      <c r="C7" s="62"/>
       <c r="D7" s="11">
         <v>0.53</v>
       </c>
@@ -8611,7 +8611,7 @@
       <c r="M7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="N7" s="42" t="s">
+      <c r="N7" s="48" t="s">
         <v>6</v>
       </c>
       <c r="O7" s="11">
@@ -8622,7 +8622,7 @@
       <c r="B8" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="46"/>
+      <c r="C8" s="63"/>
       <c r="D8" s="11">
         <v>0.51</v>
       </c>
@@ -8641,7 +8641,7 @@
       <c r="M8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="N8" s="42"/>
+      <c r="N8" s="48"/>
       <c r="O8" s="11">
         <v>1.4999999999999999E-2</v>
       </c>
@@ -8650,7 +8650,7 @@
       <c r="B9" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="44" t="s">
+      <c r="C9" s="61" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="11">
@@ -8671,7 +8671,7 @@
       <c r="M9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="N9" s="42"/>
+      <c r="N9" s="48"/>
       <c r="O9" s="11">
         <v>6.5000000000000002E-2</v>
       </c>
@@ -8680,14 +8680,14 @@
       <c r="B10" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="45"/>
+      <c r="C10" s="62"/>
       <c r="D10" s="11">
         <v>0.59</v>
       </c>
       <c r="M10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="N10" s="42"/>
+      <c r="N10" s="48"/>
       <c r="O10" s="11">
         <v>0.02</v>
       </c>
@@ -8696,14 +8696,14 @@
       <c r="B11" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="47"/>
+      <c r="C11" s="64"/>
       <c r="D11" s="13">
         <v>0.54</v>
       </c>
       <c r="M11" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="N11" s="42" t="s">
+      <c r="N11" s="48" t="s">
         <v>7</v>
       </c>
       <c r="O11" s="11">
@@ -8714,7 +8714,7 @@
       <c r="M12" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="N12" s="42"/>
+      <c r="N12" s="48"/>
       <c r="O12" s="11">
         <v>0.01</v>
       </c>
@@ -8723,7 +8723,7 @@
       <c r="M13" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="N13" s="42"/>
+      <c r="N13" s="48"/>
       <c r="O13" s="11">
         <v>5.5E-2</v>
       </c>
@@ -8732,7 +8732,7 @@
       <c r="M14" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="N14" s="43"/>
+      <c r="N14" s="49"/>
       <c r="O14" s="13">
         <v>1.4999999999999999E-2</v>
       </c>
@@ -8744,33 +8744,33 @@
       <c r="E18" s="34"/>
     </row>
     <row r="19" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C19" s="53" t="s">
+      <c r="C19" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="53"/>
+      <c r="D19" s="47"/>
       <c r="E19" s="35"/>
-      <c r="F19" s="53" t="s">
+      <c r="F19" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="G19" s="53"/>
-      <c r="I19" s="53" t="s">
+      <c r="G19" s="47"/>
+      <c r="I19" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="J19" s="53"/>
-      <c r="M19" s="57" t="s">
+      <c r="J19" s="47"/>
+      <c r="M19" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="N19" s="58"/>
-      <c r="O19" s="58"/>
-      <c r="P19" s="58"/>
-      <c r="Q19" s="58"/>
-      <c r="S19" s="59" t="s">
+      <c r="N19" s="55"/>
+      <c r="O19" s="55"/>
+      <c r="P19" s="55"/>
+      <c r="Q19" s="55"/>
+      <c r="S19" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="T19" s="60"/>
-      <c r="U19" s="60"/>
-      <c r="V19" s="60"/>
-      <c r="W19" s="60"/>
+      <c r="T19" s="57"/>
+      <c r="U19" s="57"/>
+      <c r="V19" s="57"/>
+      <c r="W19" s="57"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C20" s="16" t="s">
@@ -8792,10 +8792,10 @@
       <c r="J20" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="M20" s="54" t="s">
+      <c r="M20" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="N20" s="55"/>
+      <c r="N20" s="59"/>
       <c r="O20" s="28" t="s">
         <v>1</v>
       </c>
@@ -8805,10 +8805,10 @@
       <c r="Q20" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="S20" s="54" t="s">
+      <c r="S20" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="T20" s="55"/>
+      <c r="T20" s="59"/>
       <c r="U20" s="28" t="s">
         <v>1</v>
       </c>
@@ -8842,11 +8842,11 @@
         <f>1/(3.14*$D$4*$B$33)</f>
         <v>6.7046597385182705E-2</v>
       </c>
-      <c r="M21" s="48" t="s">
+      <c r="M21" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="N21" s="49"/>
-      <c r="O21" s="42" t="s">
+      <c r="N21" s="51"/>
+      <c r="O21" s="48" t="s">
         <v>3</v>
       </c>
       <c r="P21" s="24">
@@ -8857,11 +8857,11 @@
         <f>G27/P21</f>
         <v>6.0515045796924918</v>
       </c>
-      <c r="S21" s="48" t="s">
+      <c r="S21" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="T21" s="49"/>
-      <c r="U21" s="42" t="s">
+      <c r="T21" s="51"/>
+      <c r="U21" s="48" t="s">
         <v>3</v>
       </c>
       <c r="V21" s="24">
@@ -8896,11 +8896,11 @@
         <f>1/(3.14*$D$7*$B$33)</f>
         <v>6.3251506967153495E-2</v>
       </c>
-      <c r="M22" s="48" t="s">
+      <c r="M22" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="N22" s="49"/>
-      <c r="O22" s="42"/>
+      <c r="N22" s="51"/>
+      <c r="O22" s="48"/>
       <c r="P22" s="24">
         <f>$G$3+$G$21*$G$27^2+$O$5</f>
         <v>0.38736864523782077</v>
@@ -8909,11 +8909,11 @@
         <f>G27/P22</f>
         <v>5.2704005004016601</v>
       </c>
-      <c r="S22" s="48" t="s">
+      <c r="S22" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="T22" s="49"/>
-      <c r="U22" s="42"/>
+      <c r="T22" s="51"/>
+      <c r="U22" s="48"/>
       <c r="V22" s="24">
         <f>$G$4+$G$21*$G$27^2+$O$5</f>
         <v>0.38888164523782082</v>
@@ -8945,11 +8945,11 @@
         <f>1/(3.14*$D$10*$B$33)</f>
         <v>5.6819150326426024E-2</v>
       </c>
-      <c r="M23" s="48" t="s">
+      <c r="M23" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="N23" s="49"/>
-      <c r="O23" s="42"/>
+      <c r="N23" s="51"/>
+      <c r="O23" s="48"/>
       <c r="P23" s="24">
         <f>$G$3+$J$21*$J$27^2+$O$4</f>
         <v>0.21158435862339284</v>
@@ -8958,11 +8958,11 @@
         <f>J27/P23</f>
         <v>7.421380030644146</v>
       </c>
-      <c r="S23" s="48" t="s">
+      <c r="S23" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="T23" s="49"/>
-      <c r="U23" s="42"/>
+      <c r="T23" s="51"/>
+      <c r="U23" s="48"/>
       <c r="V23" s="24">
         <f>$G$3+$J$21*$J$27^2+$O$4</f>
         <v>0.21158435862339284</v>
@@ -8973,11 +8973,11 @@
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="M24" s="48" t="s">
+      <c r="M24" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="N24" s="49"/>
-      <c r="O24" s="42" t="s">
+      <c r="N24" s="51"/>
+      <c r="O24" s="48" t="s">
         <v>6</v>
       </c>
       <c r="P24" s="24">
@@ -8988,11 +8988,11 @@
         <f>G28/P24</f>
         <v>6.0570453985834378</v>
       </c>
-      <c r="S24" s="48" t="s">
+      <c r="S24" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="T24" s="49"/>
-      <c r="U24" s="42" t="s">
+      <c r="T24" s="51"/>
+      <c r="U24" s="48" t="s">
         <v>6</v>
       </c>
       <c r="V24" s="24">
@@ -9005,23 +9005,23 @@
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C25" s="53" t="s">
+      <c r="C25" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="53"/>
-      <c r="F25" s="53" t="s">
+      <c r="D25" s="47"/>
+      <c r="F25" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="G25" s="53"/>
-      <c r="I25" s="53" t="s">
+      <c r="G25" s="47"/>
+      <c r="I25" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="J25" s="53"/>
-      <c r="M25" s="48" t="s">
+      <c r="J25" s="47"/>
+      <c r="M25" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="N25" s="49"/>
-      <c r="O25" s="42"/>
+      <c r="N25" s="51"/>
+      <c r="O25" s="48"/>
       <c r="P25" s="24">
         <f>$G$3+$G$22*$G$28^2+$O$9</f>
         <v>0.41951114406718459</v>
@@ -9030,11 +9030,11 @@
         <f>G28/P25</f>
         <v>5.4073200056088879</v>
       </c>
-      <c r="S25" s="48" t="s">
+      <c r="S25" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="T25" s="49"/>
-      <c r="U25" s="42"/>
+      <c r="T25" s="51"/>
+      <c r="U25" s="48"/>
       <c r="V25" s="24">
         <f>$G$4+$G$22*$G$28^2+$O$9</f>
         <v>0.42102414406718464</v>
@@ -9063,11 +9063,11 @@
       <c r="J26" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="M26" s="48" t="s">
+      <c r="M26" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="N26" s="49"/>
-      <c r="O26" s="42"/>
+      <c r="N26" s="51"/>
+      <c r="O26" s="48"/>
       <c r="P26" s="24">
         <f>$G$3+$J$22*$J$28^2+$O$8</f>
         <v>0.24036489080050738</v>
@@ -9076,11 +9076,11 @@
         <f>J28/P26</f>
         <v>7.5642570432253002</v>
       </c>
-      <c r="S26" s="48" t="s">
+      <c r="S26" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="T26" s="49"/>
-      <c r="U26" s="42"/>
+      <c r="T26" s="51"/>
+      <c r="U26" s="48"/>
       <c r="V26" s="24">
         <f>$G$4+$J$22*$J$28^2+$O$8</f>
         <v>0.24187789080050737</v>
@@ -9112,11 +9112,11 @@
         <f>I7/$B$32^2</f>
         <v>1.5702479338842972</v>
       </c>
-      <c r="M27" s="48" t="s">
+      <c r="M27" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="N27" s="49"/>
-      <c r="O27" s="42" t="s">
+      <c r="N27" s="51"/>
+      <c r="O27" s="48" t="s">
         <v>7</v>
       </c>
       <c r="P27" s="24">
@@ -9127,11 +9127,11 @@
         <f>G29/P27</f>
         <v>6.1298619841834663</v>
       </c>
-      <c r="S27" s="48" t="s">
+      <c r="S27" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="T27" s="49"/>
-      <c r="U27" s="42" t="s">
+      <c r="T27" s="51"/>
+      <c r="U27" s="48" t="s">
         <v>7</v>
       </c>
       <c r="V27" s="24">
@@ -9165,11 +9165,11 @@
         <f>I8/$B$32^2</f>
         <v>1.8181818181818181</v>
       </c>
-      <c r="M28" s="48" t="s">
+      <c r="M28" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="N28" s="49"/>
-      <c r="O28" s="42"/>
+      <c r="N28" s="51"/>
+      <c r="O28" s="48"/>
       <c r="P28" s="24">
         <f>$G$3+$G$23*$G$29^2+$O$13</f>
         <v>0.43473315085935488</v>
@@ -9178,11 +9178,11 @@
         <f>G29/P28</f>
         <v>5.5658505236296705</v>
       </c>
-      <c r="S28" s="48" t="s">
+      <c r="S28" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="T28" s="49"/>
-      <c r="U28" s="42"/>
+      <c r="T28" s="51"/>
+      <c r="U28" s="48"/>
       <c r="V28" s="24">
         <f>$G$4+$G$23*$G$29^2+$O$13</f>
         <v>0.43624615085935492</v>
@@ -9214,11 +9214,11 @@
         <f>I9/$B$32^2</f>
         <v>2.0661157024793386</v>
       </c>
-      <c r="M29" s="50" t="s">
+      <c r="M29" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="N29" s="51"/>
-      <c r="O29" s="43"/>
+      <c r="N29" s="53"/>
+      <c r="O29" s="49"/>
       <c r="P29" s="27">
         <f>$G$3+$J$23*$J$29^2+$O$12</f>
         <v>0.26882052622099761</v>
@@ -9227,11 +9227,11 @@
         <f>J29/P29</f>
         <v>7.685855434940942</v>
       </c>
-      <c r="S29" s="50" t="s">
+      <c r="S29" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="T29" s="51"/>
-      <c r="U29" s="43"/>
+      <c r="T29" s="53"/>
+      <c r="U29" s="49"/>
       <c r="V29" s="27">
         <f>$G$4+$J$23*$J$29^2+$O$12</f>
         <v>0.2703335262209976</v>
@@ -9259,10 +9259,10 @@
       <c r="B31">
         <v>1.1499999999999999</v>
       </c>
-      <c r="M31" s="52" t="s">
+      <c r="M31" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="N31" s="52"/>
+      <c r="N31" s="60"/>
       <c r="O31" s="16" t="s">
         <v>22</v>
       </c>
@@ -9334,11 +9334,11 @@
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A34" s="56" t="s">
+      <c r="A34" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="56"/>
-      <c r="C34" s="56"/>
+      <c r="B34" s="46"/>
+      <c r="C34" s="46"/>
       <c r="D34" s="31"/>
       <c r="O34" s="17" t="s">
         <v>27</v>
@@ -9420,11 +9420,11 @@
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A42" s="56" t="s">
+      <c r="A42" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="56"/>
-      <c r="C42" s="56"/>
+      <c r="B42" s="46"/>
+      <c r="C42" s="46"/>
       <c r="D42" s="31"/>
       <c r="E42" t="s">
         <v>48</v>
@@ -9490,11 +9490,11 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="56" t="s">
+      <c r="A50" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="B50" s="56"/>
-      <c r="C50" s="56"/>
+      <c r="B50" s="46"/>
+      <c r="C50" s="46"/>
       <c r="D50" s="31"/>
       <c r="E50" t="s">
         <v>49</v>
@@ -9560,16 +9560,16 @@
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C57" s="61" t="s">
+      <c r="C57" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="D57" s="61"/>
-      <c r="E57" s="61"/>
-      <c r="F57" s="61" t="s">
+      <c r="D57" s="42"/>
+      <c r="E57" s="42"/>
+      <c r="F57" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="G57" s="61"/>
-      <c r="H57" s="61"/>
+      <c r="G57" s="42"/>
+      <c r="H57" s="42"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B58" s="39" t="s">
@@ -9792,16 +9792,16 @@
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C66" s="61" t="s">
+      <c r="C66" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="D66" s="61"/>
-      <c r="E66" s="61"/>
-      <c r="F66" s="62" t="s">
+      <c r="D66" s="42"/>
+      <c r="E66" s="42"/>
+      <c r="F66" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="G66" s="63"/>
-      <c r="H66" s="64"/>
+      <c r="G66" s="44"/>
+      <c r="H66" s="45"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B67" s="39" t="s">
@@ -10045,16 +10045,16 @@
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C76" s="61" t="s">
+      <c r="C76" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="D76" s="61"/>
-      <c r="E76" s="61"/>
-      <c r="F76" s="62" t="s">
+      <c r="D76" s="42"/>
+      <c r="E76" s="42"/>
+      <c r="F76" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="G76" s="63"/>
-      <c r="H76" s="64"/>
+      <c r="G76" s="44"/>
+      <c r="H76" s="45"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B77" s="39" t="s">
@@ -10299,13 +10299,33 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="C76:E76"/>
-    <mergeCell ref="F76:H76"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="F57:H57"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="N3:N6"/>
+    <mergeCell ref="N7:N10"/>
+    <mergeCell ref="N11:N14"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="S20:T20"/>
+    <mergeCell ref="S21:T21"/>
+    <mergeCell ref="S27:T27"/>
+    <mergeCell ref="O21:O23"/>
+    <mergeCell ref="O24:O26"/>
+    <mergeCell ref="O27:O29"/>
     <mergeCell ref="A34:C34"/>
     <mergeCell ref="A42:C42"/>
     <mergeCell ref="C19:D19"/>
@@ -10322,33 +10342,13 @@
     <mergeCell ref="U24:U26"/>
     <mergeCell ref="S25:T25"/>
     <mergeCell ref="S26:T26"/>
-    <mergeCell ref="S20:T20"/>
-    <mergeCell ref="S21:T21"/>
-    <mergeCell ref="S27:T27"/>
-    <mergeCell ref="O21:O23"/>
-    <mergeCell ref="O24:O26"/>
-    <mergeCell ref="O27:O29"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="M31:N31"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="N3:N6"/>
-    <mergeCell ref="N7:N10"/>
-    <mergeCell ref="N11:N14"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C76:E76"/>
+    <mergeCell ref="F76:H76"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="F57:H57"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="F66:H66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -10360,8 +10360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{381D0484-332C-4CA3-8A41-5DD9C3E4C352}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="A1:D1"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10394,8 +10394,8 @@
         <v>0.19724816049148808</v>
       </c>
       <c r="C2">
-        <f>Sheet1!$C$60</f>
-        <v>0.19724816049148808</v>
+        <f>Sheet1!$C$79</f>
+        <v>0.12920424255012972</v>
       </c>
       <c r="D2">
         <f>Sheet1!$C$69</f>
@@ -10411,8 +10411,8 @@
         <v>0.19724816049148808</v>
       </c>
       <c r="C3">
-        <f>Sheet1!$C$60</f>
-        <v>0.19724816049148808</v>
+        <f>Sheet1!$C$79</f>
+        <v>0.12920424255012972</v>
       </c>
       <c r="D3">
         <f>Sheet1!$C$69</f>
@@ -10428,8 +10428,8 @@
         <v>0.19724816049148808</v>
       </c>
       <c r="C4">
-        <f>Sheet1!$C$60</f>
-        <v>0.19724816049148808</v>
+        <f>Sheet1!$C$79</f>
+        <v>0.12920424255012972</v>
       </c>
       <c r="D4">
         <f>Sheet1!$C$69</f>
@@ -10445,8 +10445,8 @@
         <v>0.19724816049148808</v>
       </c>
       <c r="C5">
-        <f>Sheet1!$C$60</f>
-        <v>0.19724816049148808</v>
+        <f>Sheet1!$C$79</f>
+        <v>0.12920424255012972</v>
       </c>
       <c r="D5">
         <f>Sheet1!$C$69</f>
@@ -10462,8 +10462,8 @@
         <v>0.19724816049148808</v>
       </c>
       <c r="C6">
-        <f>Sheet1!$C$60</f>
-        <v>0.19724816049148808</v>
+        <f>Sheet1!$C$79</f>
+        <v>0.12920424255012972</v>
       </c>
       <c r="D6">
         <f>Sheet1!$C$69</f>
@@ -10479,8 +10479,8 @@
         <v>0.19724816049148808</v>
       </c>
       <c r="C7">
-        <f>Sheet1!$C$60</f>
-        <v>0.19724816049148808</v>
+        <f>Sheet1!$C$79</f>
+        <v>0.12920424255012972</v>
       </c>
       <c r="D7">
         <f>Sheet1!$C$69</f>
@@ -10496,8 +10496,8 @@
         <v>0.19724816049148808</v>
       </c>
       <c r="C8">
-        <f>Sheet1!$C$60</f>
-        <v>0.19724816049148808</v>
+        <f>Sheet1!$C$79</f>
+        <v>0.12920424255012972</v>
       </c>
       <c r="D8">
         <f>Sheet1!$C$69</f>
@@ -10513,8 +10513,8 @@
         <v>0.19724816049148808</v>
       </c>
       <c r="C9">
-        <f>Sheet1!$C$60</f>
-        <v>0.19724816049148808</v>
+        <f>Sheet1!$C$79</f>
+        <v>0.12920424255012972</v>
       </c>
       <c r="D9">
         <f>Sheet1!$C$69</f>
@@ -10530,8 +10530,8 @@
         <v>0.19724816049148808</v>
       </c>
       <c r="C10">
-        <f>Sheet1!$C$60</f>
-        <v>0.19724816049148808</v>
+        <f>Sheet1!$C$79</f>
+        <v>0.12920424255012972</v>
       </c>
       <c r="D10">
         <f>Sheet1!$C$69</f>
@@ -10547,8 +10547,8 @@
         <v>0.19724816049148808</v>
       </c>
       <c r="C11">
-        <f>Sheet1!$C$60</f>
-        <v>0.19724816049148808</v>
+        <f>Sheet1!$C$79</f>
+        <v>0.12920424255012972</v>
       </c>
       <c r="D11">
         <f>Sheet1!$C$69</f>
@@ -10564,8 +10564,8 @@
         <v>0.19724816049148808</v>
       </c>
       <c r="C12">
-        <f>Sheet1!$C$60</f>
-        <v>0.19724816049148808</v>
+        <f>Sheet1!$C$79</f>
+        <v>0.12920424255012972</v>
       </c>
       <c r="D12">
         <f>Sheet1!$C$69</f>
@@ -10581,8 +10581,8 @@
         <v>0.19724816049148808</v>
       </c>
       <c r="C13">
-        <f>Sheet1!$C$60</f>
-        <v>0.19724816049148808</v>
+        <f>Sheet1!$C$79</f>
+        <v>0.12920424255012972</v>
       </c>
       <c r="D13">
         <f>Sheet1!$C$69</f>
@@ -10598,8 +10598,8 @@
         <v>0.19724816049148808</v>
       </c>
       <c r="C14">
-        <f>Sheet1!$C$60</f>
-        <v>0.19724816049148808</v>
+        <f>Sheet1!$C$79</f>
+        <v>0.12920424255012972</v>
       </c>
       <c r="D14">
         <f>Sheet1!$C$69</f>
@@ -10615,8 +10615,8 @@
         <v>0.19724816049148808</v>
       </c>
       <c r="C15">
-        <f>Sheet1!$C$60</f>
-        <v>0.19724816049148808</v>
+        <f>Sheet1!$C$79</f>
+        <v>0.12920424255012972</v>
       </c>
       <c r="D15">
         <f>Sheet1!$C$69</f>
@@ -10632,8 +10632,8 @@
         <v>0.19724816049148808</v>
       </c>
       <c r="C16">
-        <f>Sheet1!$C$60</f>
-        <v>0.19724816049148808</v>
+        <f>Sheet1!$C$79</f>
+        <v>0.12920424255012972</v>
       </c>
       <c r="D16">
         <f>Sheet1!$C$69</f>
@@ -10649,8 +10649,8 @@
         <v>0.19724816049148808</v>
       </c>
       <c r="C17">
-        <f>Sheet1!$C$60</f>
-        <v>0.19724816049148808</v>
+        <f>Sheet1!$C$79</f>
+        <v>0.12920424255012972</v>
       </c>
       <c r="D17">
         <f>Sheet1!$C$69</f>
@@ -10666,8 +10666,8 @@
         <v>0.19724816049148808</v>
       </c>
       <c r="C18">
-        <f>Sheet1!$C$60</f>
-        <v>0.19724816049148808</v>
+        <f>Sheet1!$C$79</f>
+        <v>0.12920424255012972</v>
       </c>
       <c r="D18">
         <f>Sheet1!$C$69</f>
@@ -10683,8 +10683,8 @@
         <v>0.19724816049148808</v>
       </c>
       <c r="C19">
-        <f>Sheet1!$C$60</f>
-        <v>0.19724816049148808</v>
+        <f>Sheet1!$C$79</f>
+        <v>0.12920424255012972</v>
       </c>
       <c r="D19">
         <f>Sheet1!$C$69</f>
@@ -10700,8 +10700,8 @@
         <v>0.19724816049148808</v>
       </c>
       <c r="C20">
-        <f>Sheet1!$C$60</f>
-        <v>0.19724816049148808</v>
+        <f>Sheet1!$C$79</f>
+        <v>0.12920424255012972</v>
       </c>
       <c r="D20">
         <f>Sheet1!$C$69</f>
@@ -10717,8 +10717,8 @@
         <v>0.19724816049148808</v>
       </c>
       <c r="C21">
-        <f>Sheet1!$C$60</f>
-        <v>0.19724816049148808</v>
+        <f>Sheet1!$C$79</f>
+        <v>0.12920424255012972</v>
       </c>
       <c r="D21">
         <f>Sheet1!$C$69</f>
@@ -10734,8 +10734,8 @@
         <v>0.19724816049148808</v>
       </c>
       <c r="C22">
-        <f>Sheet1!$C$60</f>
-        <v>0.19724816049148808</v>
+        <f>Sheet1!$C$79</f>
+        <v>0.12920424255012972</v>
       </c>
       <c r="D22">
         <f>Sheet1!$C$69</f>
@@ -10751,8 +10751,8 @@
         <v>0.19724816049148808</v>
       </c>
       <c r="C23">
-        <f>Sheet1!$C$60</f>
-        <v>0.19724816049148808</v>
+        <f>Sheet1!$C$79</f>
+        <v>0.12920424255012972</v>
       </c>
       <c r="D23">
         <f>Sheet1!$C$69</f>
@@ -10768,8 +10768,8 @@
         <v>0.19724816049148808</v>
       </c>
       <c r="C24">
-        <f>Sheet1!$C$60</f>
-        <v>0.19724816049148808</v>
+        <f>Sheet1!$C$79</f>
+        <v>0.12920424255012972</v>
       </c>
       <c r="D24">
         <f>Sheet1!$C$69</f>
@@ -10785,8 +10785,8 @@
         <v>0.19724816049148808</v>
       </c>
       <c r="C25">
-        <f>Sheet1!$C$60</f>
-        <v>0.19724816049148808</v>
+        <f>Sheet1!$C$79</f>
+        <v>0.12920424255012972</v>
       </c>
       <c r="D25">
         <f>Sheet1!$C$69</f>
@@ -10802,8 +10802,8 @@
         <v>0.19724816049148808</v>
       </c>
       <c r="C26">
-        <f>Sheet1!$C$60</f>
-        <v>0.19724816049148808</v>
+        <f>Sheet1!$C$79</f>
+        <v>0.12920424255012972</v>
       </c>
       <c r="D26">
         <f>Sheet1!$C$69</f>
@@ -10819,8 +10819,8 @@
         <v>0.19724816049148808</v>
       </c>
       <c r="C27">
-        <f>Sheet1!$C$60</f>
-        <v>0.19724816049148808</v>
+        <f>Sheet1!$C$79</f>
+        <v>0.12920424255012972</v>
       </c>
       <c r="D27">
         <f>Sheet1!$C$69</f>
@@ -10836,8 +10836,8 @@
         <v>0.19724816049148808</v>
       </c>
       <c r="C28">
-        <f>Sheet1!$C$60</f>
-        <v>0.19724816049148808</v>
+        <f>Sheet1!$C$79</f>
+        <v>0.12920424255012972</v>
       </c>
       <c r="D28">
         <f>Sheet1!$C$69</f>
@@ -10853,8 +10853,8 @@
         <v>0.19724816049148808</v>
       </c>
       <c r="C29">
-        <f>Sheet1!$C$60</f>
-        <v>0.19724816049148808</v>
+        <f>Sheet1!$C$79</f>
+        <v>0.12920424255012972</v>
       </c>
       <c r="D29">
         <f>Sheet1!$C$69</f>
@@ -10870,8 +10870,8 @@
         <v>0.19724816049148808</v>
       </c>
       <c r="C30">
-        <f>Sheet1!$C$60</f>
-        <v>0.19724816049148808</v>
+        <f>Sheet1!$C$79</f>
+        <v>0.12920424255012972</v>
       </c>
       <c r="D30">
         <f>Sheet1!$C$69</f>
@@ -10887,8 +10887,8 @@
         <v>0.19724816049148808</v>
       </c>
       <c r="C31">
-        <f>Sheet1!$C$60</f>
-        <v>0.19724816049148808</v>
+        <f>Sheet1!$C$79</f>
+        <v>0.12920424255012972</v>
       </c>
       <c r="D31">
         <f>Sheet1!$C$69</f>
@@ -10904,8 +10904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7912584B-6A7A-4607-AF47-DB00BC4FE5B9}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10938,8 +10938,8 @@
         <v>0.19709699600961719</v>
       </c>
       <c r="C2">
-        <f>Sheet1!$D$60</f>
-        <v>0.19709699600961719</v>
+        <f>Sheet1!$D$79</f>
+        <v>0.13584532727168921</v>
       </c>
       <c r="D2">
         <f>Sheet1!$D$69</f>
@@ -10955,8 +10955,8 @@
         <v>0.19709699600961719</v>
       </c>
       <c r="C3">
-        <f>Sheet1!$D$60</f>
-        <v>0.19709699600961719</v>
+        <f>Sheet1!$D$79</f>
+        <v>0.13584532727168921</v>
       </c>
       <c r="D3">
         <f>Sheet1!$D$69</f>
@@ -10972,8 +10972,8 @@
         <v>0.19709699600961719</v>
       </c>
       <c r="C4">
-        <f>Sheet1!$D$60</f>
-        <v>0.19709699600961719</v>
+        <f>Sheet1!$D$79</f>
+        <v>0.13584532727168921</v>
       </c>
       <c r="D4">
         <f>Sheet1!$D$69</f>
@@ -10989,8 +10989,8 @@
         <v>0.19709699600961719</v>
       </c>
       <c r="C5">
-        <f>Sheet1!$D$60</f>
-        <v>0.19709699600961719</v>
+        <f>Sheet1!$D$79</f>
+        <v>0.13584532727168921</v>
       </c>
       <c r="D5">
         <f>Sheet1!$D$69</f>
@@ -11006,8 +11006,8 @@
         <v>0.19709699600961719</v>
       </c>
       <c r="C6">
-        <f>Sheet1!$D$60</f>
-        <v>0.19709699600961719</v>
+        <f>Sheet1!$D$79</f>
+        <v>0.13584532727168921</v>
       </c>
       <c r="D6">
         <f>Sheet1!$D$69</f>
@@ -11023,8 +11023,8 @@
         <v>0.19709699600961719</v>
       </c>
       <c r="C7">
-        <f>Sheet1!$D$60</f>
-        <v>0.19709699600961719</v>
+        <f>Sheet1!$D$79</f>
+        <v>0.13584532727168921</v>
       </c>
       <c r="D7">
         <f>Sheet1!$D$69</f>
@@ -11040,8 +11040,8 @@
         <v>0.19709699600961719</v>
       </c>
       <c r="C8">
-        <f>Sheet1!$D$60</f>
-        <v>0.19709699600961719</v>
+        <f>Sheet1!$D$79</f>
+        <v>0.13584532727168921</v>
       </c>
       <c r="D8">
         <f>Sheet1!$D$69</f>
@@ -11057,8 +11057,8 @@
         <v>0.19709699600961719</v>
       </c>
       <c r="C9">
-        <f>Sheet1!$D$60</f>
-        <v>0.19709699600961719</v>
+        <f>Sheet1!$D$79</f>
+        <v>0.13584532727168921</v>
       </c>
       <c r="D9">
         <f>Sheet1!$D$69</f>
@@ -11074,8 +11074,8 @@
         <v>0.19709699600961719</v>
       </c>
       <c r="C10">
-        <f>Sheet1!$D$60</f>
-        <v>0.19709699600961719</v>
+        <f>Sheet1!$D$79</f>
+        <v>0.13584532727168921</v>
       </c>
       <c r="D10">
         <f>Sheet1!$D$69</f>
@@ -11091,8 +11091,8 @@
         <v>0.19709699600961719</v>
       </c>
       <c r="C11">
-        <f>Sheet1!$D$60</f>
-        <v>0.19709699600961719</v>
+        <f>Sheet1!$D$79</f>
+        <v>0.13584532727168921</v>
       </c>
       <c r="D11">
         <f>Sheet1!$D$69</f>
@@ -11108,8 +11108,8 @@
         <v>0.19709699600961719</v>
       </c>
       <c r="C12">
-        <f>Sheet1!$D$60</f>
-        <v>0.19709699600961719</v>
+        <f>Sheet1!$D$79</f>
+        <v>0.13584532727168921</v>
       </c>
       <c r="D12">
         <f>Sheet1!$D$69</f>
@@ -11125,8 +11125,8 @@
         <v>0.19709699600961719</v>
       </c>
       <c r="C13">
-        <f>Sheet1!$D$60</f>
-        <v>0.19709699600961719</v>
+        <f>Sheet1!$D$79</f>
+        <v>0.13584532727168921</v>
       </c>
       <c r="D13">
         <f>Sheet1!$D$69</f>
@@ -11142,8 +11142,8 @@
         <v>0.19709699600961719</v>
       </c>
       <c r="C14">
-        <f>Sheet1!$D$60</f>
-        <v>0.19709699600961719</v>
+        <f>Sheet1!$D$79</f>
+        <v>0.13584532727168921</v>
       </c>
       <c r="D14">
         <f>Sheet1!$D$69</f>
@@ -11159,8 +11159,8 @@
         <v>0.19709699600961719</v>
       </c>
       <c r="C15">
-        <f>Sheet1!$D$60</f>
-        <v>0.19709699600961719</v>
+        <f>Sheet1!$D$79</f>
+        <v>0.13584532727168921</v>
       </c>
       <c r="D15">
         <f>Sheet1!$D$69</f>
@@ -11176,8 +11176,8 @@
         <v>0.19709699600961719</v>
       </c>
       <c r="C16">
-        <f>Sheet1!$D$60</f>
-        <v>0.19709699600961719</v>
+        <f>Sheet1!$D$79</f>
+        <v>0.13584532727168921</v>
       </c>
       <c r="D16">
         <f>Sheet1!$D$69</f>
@@ -11193,8 +11193,8 @@
         <v>0.19709699600961719</v>
       </c>
       <c r="C17">
-        <f>Sheet1!$D$60</f>
-        <v>0.19709699600961719</v>
+        <f>Sheet1!$D$79</f>
+        <v>0.13584532727168921</v>
       </c>
       <c r="D17">
         <f>Sheet1!$D$69</f>
@@ -11210,8 +11210,8 @@
         <v>0.19709699600961719</v>
       </c>
       <c r="C18">
-        <f>Sheet1!$D$60</f>
-        <v>0.19709699600961719</v>
+        <f>Sheet1!$D$79</f>
+        <v>0.13584532727168921</v>
       </c>
       <c r="D18">
         <f>Sheet1!$D$69</f>
@@ -11227,8 +11227,8 @@
         <v>0.19709699600961719</v>
       </c>
       <c r="C19">
-        <f>Sheet1!$D$60</f>
-        <v>0.19709699600961719</v>
+        <f>Sheet1!$D$79</f>
+        <v>0.13584532727168921</v>
       </c>
       <c r="D19">
         <f>Sheet1!$D$69</f>
@@ -11244,8 +11244,8 @@
         <v>0.19709699600961719</v>
       </c>
       <c r="C20">
-        <f>Sheet1!$D$60</f>
-        <v>0.19709699600961719</v>
+        <f>Sheet1!$D$79</f>
+        <v>0.13584532727168921</v>
       </c>
       <c r="D20">
         <f>Sheet1!$D$69</f>
@@ -11261,8 +11261,8 @@
         <v>0.19709699600961719</v>
       </c>
       <c r="C21">
-        <f>Sheet1!$D$60</f>
-        <v>0.19709699600961719</v>
+        <f>Sheet1!$D$79</f>
+        <v>0.13584532727168921</v>
       </c>
       <c r="D21">
         <f>Sheet1!$D$69</f>
@@ -11278,8 +11278,8 @@
         <v>0.19709699600961719</v>
       </c>
       <c r="C22">
-        <f>Sheet1!$D$60</f>
-        <v>0.19709699600961719</v>
+        <f>Sheet1!$D$79</f>
+        <v>0.13584532727168921</v>
       </c>
       <c r="D22">
         <f>Sheet1!$D$69</f>
@@ -11295,8 +11295,8 @@
         <v>0.19709699600961719</v>
       </c>
       <c r="C23">
-        <f>Sheet1!$D$60</f>
-        <v>0.19709699600961719</v>
+        <f>Sheet1!$D$79</f>
+        <v>0.13584532727168921</v>
       </c>
       <c r="D23">
         <f>Sheet1!$D$69</f>
@@ -11312,8 +11312,8 @@
         <v>0.19709699600961719</v>
       </c>
       <c r="C24">
-        <f>Sheet1!$D$60</f>
-        <v>0.19709699600961719</v>
+        <f>Sheet1!$D$79</f>
+        <v>0.13584532727168921</v>
       </c>
       <c r="D24">
         <f>Sheet1!$D$69</f>
@@ -11329,8 +11329,8 @@
         <v>0.19709699600961719</v>
       </c>
       <c r="C25">
-        <f>Sheet1!$D$60</f>
-        <v>0.19709699600961719</v>
+        <f>Sheet1!$D$79</f>
+        <v>0.13584532727168921</v>
       </c>
       <c r="D25">
         <f>Sheet1!$D$69</f>
@@ -11346,8 +11346,8 @@
         <v>0.19709699600961719</v>
       </c>
       <c r="C26">
-        <f>Sheet1!$D$60</f>
-        <v>0.19709699600961719</v>
+        <f>Sheet1!$D$79</f>
+        <v>0.13584532727168921</v>
       </c>
       <c r="D26">
         <f>Sheet1!$D$69</f>
@@ -11363,8 +11363,8 @@
         <v>0.19709699600961719</v>
       </c>
       <c r="C27">
-        <f>Sheet1!$D$60</f>
-        <v>0.19709699600961719</v>
+        <f>Sheet1!$D$79</f>
+        <v>0.13584532727168921</v>
       </c>
       <c r="D27">
         <f>Sheet1!$D$69</f>
@@ -11380,8 +11380,8 @@
         <v>0.19709699600961719</v>
       </c>
       <c r="C28">
-        <f>Sheet1!$D$60</f>
-        <v>0.19709699600961719</v>
+        <f>Sheet1!$D$79</f>
+        <v>0.13584532727168921</v>
       </c>
       <c r="D28">
         <f>Sheet1!$D$69</f>
@@ -11397,8 +11397,8 @@
         <v>0.19709699600961719</v>
       </c>
       <c r="C29">
-        <f>Sheet1!$D$60</f>
-        <v>0.19709699600961719</v>
+        <f>Sheet1!$D$79</f>
+        <v>0.13584532727168921</v>
       </c>
       <c r="D29">
         <f>Sheet1!$D$69</f>
@@ -11414,8 +11414,8 @@
         <v>0.19709699600961719</v>
       </c>
       <c r="C30">
-        <f>Sheet1!$D$60</f>
-        <v>0.19709699600961719</v>
+        <f>Sheet1!$D$79</f>
+        <v>0.13584532727168921</v>
       </c>
       <c r="D30">
         <f>Sheet1!$D$69</f>
@@ -11431,8 +11431,8 @@
         <v>0.19709699600961719</v>
       </c>
       <c r="C31">
-        <f>Sheet1!$D$60</f>
-        <v>0.19709699600961719</v>
+        <f>Sheet1!$D$79</f>
+        <v>0.13584532727168921</v>
       </c>
       <c r="D31">
         <f>Sheet1!$D$69</f>
@@ -11448,8 +11448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9953794-7C51-4E00-859A-523BF6F04AB5}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11482,8 +11482,8 @@
         <v>0.19513581000359276</v>
       </c>
       <c r="C2">
-        <f>Sheet1!$E$60</f>
-        <v>0.19513581000359276</v>
+        <f>Sheet1!$E$79</f>
+        <v>0.14593872489654086</v>
       </c>
       <c r="D2">
         <f>Sheet1!$E$69</f>
@@ -11499,8 +11499,8 @@
         <v>0.19513581000359276</v>
       </c>
       <c r="C3">
-        <f>Sheet1!$E$60</f>
-        <v>0.19513581000359276</v>
+        <f>Sheet1!$E$79</f>
+        <v>0.14593872489654086</v>
       </c>
       <c r="D3">
         <f>Sheet1!$E$69</f>
@@ -11516,8 +11516,8 @@
         <v>0.19513581000359276</v>
       </c>
       <c r="C4">
-        <f>Sheet1!$E$60</f>
-        <v>0.19513581000359276</v>
+        <f>Sheet1!$E$79</f>
+        <v>0.14593872489654086</v>
       </c>
       <c r="D4">
         <f>Sheet1!$E$69</f>
@@ -11533,8 +11533,8 @@
         <v>0.19513581000359276</v>
       </c>
       <c r="C5">
-        <f>Sheet1!$E$60</f>
-        <v>0.19513581000359276</v>
+        <f>Sheet1!$E$79</f>
+        <v>0.14593872489654086</v>
       </c>
       <c r="D5">
         <f>Sheet1!$E$69</f>
@@ -11550,8 +11550,8 @@
         <v>0.19513581000359276</v>
       </c>
       <c r="C6">
-        <f>Sheet1!$E$60</f>
-        <v>0.19513581000359276</v>
+        <f>Sheet1!$E$79</f>
+        <v>0.14593872489654086</v>
       </c>
       <c r="D6">
         <f>Sheet1!$E$69</f>
@@ -11567,8 +11567,8 @@
         <v>0.19513581000359276</v>
       </c>
       <c r="C7">
-        <f>Sheet1!$E$60</f>
-        <v>0.19513581000359276</v>
+        <f>Sheet1!$E$79</f>
+        <v>0.14593872489654086</v>
       </c>
       <c r="D7">
         <f>Sheet1!$E$69</f>
@@ -11584,8 +11584,8 @@
         <v>0.19513581000359276</v>
       </c>
       <c r="C8">
-        <f>Sheet1!$E$60</f>
-        <v>0.19513581000359276</v>
+        <f>Sheet1!$E$79</f>
+        <v>0.14593872489654086</v>
       </c>
       <c r="D8">
         <f>Sheet1!$E$69</f>
@@ -11601,8 +11601,8 @@
         <v>0.19513581000359276</v>
       </c>
       <c r="C9">
-        <f>Sheet1!$E$60</f>
-        <v>0.19513581000359276</v>
+        <f>Sheet1!$E$79</f>
+        <v>0.14593872489654086</v>
       </c>
       <c r="D9">
         <f>Sheet1!$E$69</f>
@@ -11618,8 +11618,8 @@
         <v>0.19513581000359276</v>
       </c>
       <c r="C10">
-        <f>Sheet1!$E$60</f>
-        <v>0.19513581000359276</v>
+        <f>Sheet1!$E$79</f>
+        <v>0.14593872489654086</v>
       </c>
       <c r="D10">
         <f>Sheet1!$E$69</f>
@@ -11635,8 +11635,8 @@
         <v>0.19513581000359276</v>
       </c>
       <c r="C11">
-        <f>Sheet1!$E$60</f>
-        <v>0.19513581000359276</v>
+        <f>Sheet1!$E$79</f>
+        <v>0.14593872489654086</v>
       </c>
       <c r="D11">
         <f>Sheet1!$E$69</f>
@@ -11652,8 +11652,8 @@
         <v>0.19513581000359276</v>
       </c>
       <c r="C12">
-        <f>Sheet1!$E$60</f>
-        <v>0.19513581000359276</v>
+        <f>Sheet1!$E$79</f>
+        <v>0.14593872489654086</v>
       </c>
       <c r="D12">
         <f>Sheet1!$E$69</f>
@@ -11669,8 +11669,8 @@
         <v>0.19513581000359276</v>
       </c>
       <c r="C13">
-        <f>Sheet1!$E$60</f>
-        <v>0.19513581000359276</v>
+        <f>Sheet1!$E$79</f>
+        <v>0.14593872489654086</v>
       </c>
       <c r="D13">
         <f>Sheet1!$E$69</f>
@@ -11686,8 +11686,8 @@
         <v>0.19513581000359276</v>
       </c>
       <c r="C14">
-        <f>Sheet1!$E$60</f>
-        <v>0.19513581000359276</v>
+        <f>Sheet1!$E$79</f>
+        <v>0.14593872489654086</v>
       </c>
       <c r="D14">
         <f>Sheet1!$E$69</f>
@@ -11703,8 +11703,8 @@
         <v>0.19513581000359276</v>
       </c>
       <c r="C15">
-        <f>Sheet1!$E$60</f>
-        <v>0.19513581000359276</v>
+        <f>Sheet1!$E$79</f>
+        <v>0.14593872489654086</v>
       </c>
       <c r="D15">
         <f>Sheet1!$E$69</f>
@@ -11720,8 +11720,8 @@
         <v>0.19513581000359276</v>
       </c>
       <c r="C16">
-        <f>Sheet1!$E$60</f>
-        <v>0.19513581000359276</v>
+        <f>Sheet1!$E$79</f>
+        <v>0.14593872489654086</v>
       </c>
       <c r="D16">
         <f>Sheet1!$E$69</f>
@@ -11737,8 +11737,8 @@
         <v>0.19513581000359276</v>
       </c>
       <c r="C17">
-        <f>Sheet1!$E$60</f>
-        <v>0.19513581000359276</v>
+        <f>Sheet1!$E$79</f>
+        <v>0.14593872489654086</v>
       </c>
       <c r="D17">
         <f>Sheet1!$E$69</f>
@@ -11754,8 +11754,8 @@
         <v>0.19513581000359276</v>
       </c>
       <c r="C18">
-        <f>Sheet1!$E$60</f>
-        <v>0.19513581000359276</v>
+        <f>Sheet1!$E$79</f>
+        <v>0.14593872489654086</v>
       </c>
       <c r="D18">
         <f>Sheet1!$E$69</f>
@@ -11771,8 +11771,8 @@
         <v>0.19513581000359276</v>
       </c>
       <c r="C19">
-        <f>Sheet1!$E$60</f>
-        <v>0.19513581000359276</v>
+        <f>Sheet1!$E$79</f>
+        <v>0.14593872489654086</v>
       </c>
       <c r="D19">
         <f>Sheet1!$E$69</f>
@@ -11788,8 +11788,8 @@
         <v>0.19513581000359276</v>
       </c>
       <c r="C20">
-        <f>Sheet1!$E$60</f>
-        <v>0.19513581000359276</v>
+        <f>Sheet1!$E$79</f>
+        <v>0.14593872489654086</v>
       </c>
       <c r="D20">
         <f>Sheet1!$E$69</f>
@@ -11805,8 +11805,8 @@
         <v>0.19513581000359276</v>
       </c>
       <c r="C21">
-        <f>Sheet1!$E$60</f>
-        <v>0.19513581000359276</v>
+        <f>Sheet1!$E$79</f>
+        <v>0.14593872489654086</v>
       </c>
       <c r="D21">
         <f>Sheet1!$E$69</f>
@@ -11822,8 +11822,8 @@
         <v>0.19513581000359276</v>
       </c>
       <c r="C22">
-        <f>Sheet1!$E$60</f>
-        <v>0.19513581000359276</v>
+        <f>Sheet1!$E$79</f>
+        <v>0.14593872489654086</v>
       </c>
       <c r="D22">
         <f>Sheet1!$E$69</f>
@@ -11839,8 +11839,8 @@
         <v>0.19513581000359276</v>
       </c>
       <c r="C23">
-        <f>Sheet1!$E$60</f>
-        <v>0.19513581000359276</v>
+        <f>Sheet1!$E$79</f>
+        <v>0.14593872489654086</v>
       </c>
       <c r="D23">
         <f>Sheet1!$E$69</f>
@@ -11856,8 +11856,8 @@
         <v>0.19513581000359276</v>
       </c>
       <c r="C24">
-        <f>Sheet1!$E$60</f>
-        <v>0.19513581000359276</v>
+        <f>Sheet1!$E$79</f>
+        <v>0.14593872489654086</v>
       </c>
       <c r="D24">
         <f>Sheet1!$E$69</f>
@@ -11873,8 +11873,8 @@
         <v>0.19513581000359276</v>
       </c>
       <c r="C25">
-        <f>Sheet1!$E$60</f>
-        <v>0.19513581000359276</v>
+        <f>Sheet1!$E$79</f>
+        <v>0.14593872489654086</v>
       </c>
       <c r="D25">
         <f>Sheet1!$E$69</f>
@@ -11890,8 +11890,8 @@
         <v>0.19513581000359276</v>
       </c>
       <c r="C26">
-        <f>Sheet1!$E$60</f>
-        <v>0.19513581000359276</v>
+        <f>Sheet1!$E$79</f>
+        <v>0.14593872489654086</v>
       </c>
       <c r="D26">
         <f>Sheet1!$E$69</f>
@@ -11907,8 +11907,8 @@
         <v>0.19513581000359276</v>
       </c>
       <c r="C27">
-        <f>Sheet1!$E$60</f>
-        <v>0.19513581000359276</v>
+        <f>Sheet1!$E$79</f>
+        <v>0.14593872489654086</v>
       </c>
       <c r="D27">
         <f>Sheet1!$E$69</f>
@@ -11924,8 +11924,8 @@
         <v>0.19513581000359276</v>
       </c>
       <c r="C28">
-        <f>Sheet1!$E$60</f>
-        <v>0.19513581000359276</v>
+        <f>Sheet1!$E$79</f>
+        <v>0.14593872489654086</v>
       </c>
       <c r="D28">
         <f>Sheet1!$E$69</f>
@@ -11941,8 +11941,8 @@
         <v>0.19513581000359276</v>
       </c>
       <c r="C29">
-        <f>Sheet1!$E$60</f>
-        <v>0.19513581000359276</v>
+        <f>Sheet1!$E$79</f>
+        <v>0.14593872489654086</v>
       </c>
       <c r="D29">
         <f>Sheet1!$E$69</f>
@@ -11958,8 +11958,8 @@
         <v>0.19513581000359276</v>
       </c>
       <c r="C30">
-        <f>Sheet1!$E$60</f>
-        <v>0.19513581000359276</v>
+        <f>Sheet1!$E$79</f>
+        <v>0.14593872489654086</v>
       </c>
       <c r="D30">
         <f>Sheet1!$E$69</f>
@@ -11975,8 +11975,8 @@
         <v>0.19513581000359276</v>
       </c>
       <c r="C31">
-        <f>Sheet1!$E$60</f>
-        <v>0.19513581000359276</v>
+        <f>Sheet1!$E$79</f>
+        <v>0.14593872489654086</v>
       </c>
       <c r="D31">
         <f>Sheet1!$E$69</f>
@@ -11992,8 +11992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0656B60B-719F-400A-BE92-F6DEDEF6288E}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12026,8 +12026,8 @@
         <v>0.19798925030630293</v>
       </c>
       <c r="C2">
-        <f>Sheet1!$F$60</f>
-        <v>0.19798925030630293</v>
+        <f>Sheet1!$F$79</f>
+        <v>0.13216860180938897</v>
       </c>
       <c r="D2">
         <f>Sheet1!$F$69</f>
@@ -12043,8 +12043,8 @@
         <v>0.19798925030630293</v>
       </c>
       <c r="C3">
-        <f>Sheet1!$F$60</f>
-        <v>0.19798925030630293</v>
+        <f>Sheet1!$F$79</f>
+        <v>0.13216860180938897</v>
       </c>
       <c r="D3">
         <f>Sheet1!$F$69</f>
@@ -12060,8 +12060,8 @@
         <v>0.19798925030630293</v>
       </c>
       <c r="C4">
-        <f>Sheet1!$F$60</f>
-        <v>0.19798925030630293</v>
+        <f>Sheet1!$F$79</f>
+        <v>0.13216860180938897</v>
       </c>
       <c r="D4">
         <f>Sheet1!$F$69</f>
@@ -12077,8 +12077,8 @@
         <v>0.19798925030630293</v>
       </c>
       <c r="C5">
-        <f>Sheet1!$F$60</f>
-        <v>0.19798925030630293</v>
+        <f>Sheet1!$F$79</f>
+        <v>0.13216860180938897</v>
       </c>
       <c r="D5">
         <f>Sheet1!$F$69</f>
@@ -12094,8 +12094,8 @@
         <v>0.19798925030630293</v>
       </c>
       <c r="C6">
-        <f>Sheet1!$F$60</f>
-        <v>0.19798925030630293</v>
+        <f>Sheet1!$F$79</f>
+        <v>0.13216860180938897</v>
       </c>
       <c r="D6">
         <f>Sheet1!$F$69</f>
@@ -12111,8 +12111,8 @@
         <v>0.19798925030630293</v>
       </c>
       <c r="C7">
-        <f>Sheet1!$F$60</f>
-        <v>0.19798925030630293</v>
+        <f>Sheet1!$F$79</f>
+        <v>0.13216860180938897</v>
       </c>
       <c r="D7">
         <f>Sheet1!$F$69</f>
@@ -12128,8 +12128,8 @@
         <v>0.19798925030630293</v>
       </c>
       <c r="C8">
-        <f>Sheet1!$F$60</f>
-        <v>0.19798925030630293</v>
+        <f>Sheet1!$F$79</f>
+        <v>0.13216860180938897</v>
       </c>
       <c r="D8">
         <f>Sheet1!$F$69</f>
@@ -12145,8 +12145,8 @@
         <v>0.19798925030630293</v>
       </c>
       <c r="C9">
-        <f>Sheet1!$F$60</f>
-        <v>0.19798925030630293</v>
+        <f>Sheet1!$F$79</f>
+        <v>0.13216860180938897</v>
       </c>
       <c r="D9">
         <f>Sheet1!$F$69</f>
@@ -12162,8 +12162,8 @@
         <v>0.19798925030630293</v>
       </c>
       <c r="C10">
-        <f>Sheet1!$F$60</f>
-        <v>0.19798925030630293</v>
+        <f>Sheet1!$F$79</f>
+        <v>0.13216860180938897</v>
       </c>
       <c r="D10">
         <f>Sheet1!$F$69</f>
@@ -12179,8 +12179,8 @@
         <v>0.19798925030630293</v>
       </c>
       <c r="C11">
-        <f>Sheet1!$F$60</f>
-        <v>0.19798925030630293</v>
+        <f>Sheet1!$F$79</f>
+        <v>0.13216860180938897</v>
       </c>
       <c r="D11">
         <f>Sheet1!$F$69</f>
@@ -12196,8 +12196,8 @@
         <v>0.19798925030630293</v>
       </c>
       <c r="C12">
-        <f>Sheet1!$F$60</f>
-        <v>0.19798925030630293</v>
+        <f>Sheet1!$F$79</f>
+        <v>0.13216860180938897</v>
       </c>
       <c r="D12">
         <f>Sheet1!$F$69</f>
@@ -12213,8 +12213,8 @@
         <v>0.19798925030630293</v>
       </c>
       <c r="C13">
-        <f>Sheet1!$F$60</f>
-        <v>0.19798925030630293</v>
+        <f>Sheet1!$F$79</f>
+        <v>0.13216860180938897</v>
       </c>
       <c r="D13">
         <f>Sheet1!$F$69</f>
@@ -12230,8 +12230,8 @@
         <v>0.19798925030630293</v>
       </c>
       <c r="C14">
-        <f>Sheet1!$F$60</f>
-        <v>0.19798925030630293</v>
+        <f>Sheet1!$F$79</f>
+        <v>0.13216860180938897</v>
       </c>
       <c r="D14">
         <f>Sheet1!$F$69</f>
@@ -12247,8 +12247,8 @@
         <v>0.19798925030630293</v>
       </c>
       <c r="C15">
-        <f>Sheet1!$F$60</f>
-        <v>0.19798925030630293</v>
+        <f>Sheet1!$F$79</f>
+        <v>0.13216860180938897</v>
       </c>
       <c r="D15">
         <f>Sheet1!$F$69</f>
@@ -12264,8 +12264,8 @@
         <v>0.19798925030630293</v>
       </c>
       <c r="C16">
-        <f>Sheet1!$F$60</f>
-        <v>0.19798925030630293</v>
+        <f>Sheet1!$F$79</f>
+        <v>0.13216860180938897</v>
       </c>
       <c r="D16">
         <f>Sheet1!$F$69</f>
@@ -12281,8 +12281,8 @@
         <v>0.19798925030630293</v>
       </c>
       <c r="C17">
-        <f>Sheet1!$F$60</f>
-        <v>0.19798925030630293</v>
+        <f>Sheet1!$F$79</f>
+        <v>0.13216860180938897</v>
       </c>
       <c r="D17">
         <f>Sheet1!$F$69</f>
@@ -12298,8 +12298,8 @@
         <v>0.19798925030630293</v>
       </c>
       <c r="C18">
-        <f>Sheet1!$F$60</f>
-        <v>0.19798925030630293</v>
+        <f>Sheet1!$F$79</f>
+        <v>0.13216860180938897</v>
       </c>
       <c r="D18">
         <f>Sheet1!$F$69</f>
@@ -12315,8 +12315,8 @@
         <v>0.19798925030630293</v>
       </c>
       <c r="C19">
-        <f>Sheet1!$F$60</f>
-        <v>0.19798925030630293</v>
+        <f>Sheet1!$F$79</f>
+        <v>0.13216860180938897</v>
       </c>
       <c r="D19">
         <f>Sheet1!$F$69</f>
@@ -12332,8 +12332,8 @@
         <v>0.19798925030630293</v>
       </c>
       <c r="C20">
-        <f>Sheet1!$F$60</f>
-        <v>0.19798925030630293</v>
+        <f>Sheet1!$F$79</f>
+        <v>0.13216860180938897</v>
       </c>
       <c r="D20">
         <f>Sheet1!$F$69</f>
@@ -12349,8 +12349,8 @@
         <v>0.19798925030630293</v>
       </c>
       <c r="C21">
-        <f>Sheet1!$F$60</f>
-        <v>0.19798925030630293</v>
+        <f>Sheet1!$F$79</f>
+        <v>0.13216860180938897</v>
       </c>
       <c r="D21">
         <f>Sheet1!$F$69</f>
@@ -12366,8 +12366,8 @@
         <v>0.19798925030630293</v>
       </c>
       <c r="C22">
-        <f>Sheet1!$F$60</f>
-        <v>0.19798925030630293</v>
+        <f>Sheet1!$F$79</f>
+        <v>0.13216860180938897</v>
       </c>
       <c r="D22">
         <f>Sheet1!$F$69</f>
@@ -12383,8 +12383,8 @@
         <v>0.19798925030630293</v>
       </c>
       <c r="C23">
-        <f>Sheet1!$F$60</f>
-        <v>0.19798925030630293</v>
+        <f>Sheet1!$F$79</f>
+        <v>0.13216860180938897</v>
       </c>
       <c r="D23">
         <f>Sheet1!$F$69</f>
@@ -12400,8 +12400,8 @@
         <v>0.19798925030630293</v>
       </c>
       <c r="C24">
-        <f>Sheet1!$F$60</f>
-        <v>0.19798925030630293</v>
+        <f>Sheet1!$F$79</f>
+        <v>0.13216860180938897</v>
       </c>
       <c r="D24">
         <f>Sheet1!$F$69</f>
@@ -12417,8 +12417,8 @@
         <v>0.19798925030630293</v>
       </c>
       <c r="C25">
-        <f>Sheet1!$F$60</f>
-        <v>0.19798925030630293</v>
+        <f>Sheet1!$F$79</f>
+        <v>0.13216860180938897</v>
       </c>
       <c r="D25">
         <f>Sheet1!$F$69</f>
@@ -12434,8 +12434,8 @@
         <v>0.19798925030630293</v>
       </c>
       <c r="C26">
-        <f>Sheet1!$F$60</f>
-        <v>0.19798925030630293</v>
+        <f>Sheet1!$F$79</f>
+        <v>0.13216860180938897</v>
       </c>
       <c r="D26">
         <f>Sheet1!$F$69</f>
@@ -12451,8 +12451,8 @@
         <v>0.19798925030630293</v>
       </c>
       <c r="C27">
-        <f>Sheet1!$F$60</f>
-        <v>0.19798925030630293</v>
+        <f>Sheet1!$F$79</f>
+        <v>0.13216860180938897</v>
       </c>
       <c r="D27">
         <f>Sheet1!$F$69</f>
@@ -12468,8 +12468,8 @@
         <v>0.19798925030630293</v>
       </c>
       <c r="C28">
-        <f>Sheet1!$F$60</f>
-        <v>0.19798925030630293</v>
+        <f>Sheet1!$F$79</f>
+        <v>0.13216860180938897</v>
       </c>
       <c r="D28">
         <f>Sheet1!$F$69</f>
@@ -12485,8 +12485,8 @@
         <v>0.19798925030630293</v>
       </c>
       <c r="C29">
-        <f>Sheet1!$F$60</f>
-        <v>0.19798925030630293</v>
+        <f>Sheet1!$F$79</f>
+        <v>0.13216860180938897</v>
       </c>
       <c r="D29">
         <f>Sheet1!$F$69</f>
@@ -12502,8 +12502,8 @@
         <v>0.19798925030630293</v>
       </c>
       <c r="C30">
-        <f>Sheet1!$F$60</f>
-        <v>0.19798925030630293</v>
+        <f>Sheet1!$F$79</f>
+        <v>0.13216860180938897</v>
       </c>
       <c r="D30">
         <f>Sheet1!$F$69</f>
@@ -12519,8 +12519,8 @@
         <v>0.19798925030630293</v>
       </c>
       <c r="C31">
-        <f>Sheet1!$F$60</f>
-        <v>0.19798925030630293</v>
+        <f>Sheet1!$F$79</f>
+        <v>0.13216860180938897</v>
       </c>
       <c r="D31">
         <f>Sheet1!$F$69</f>
@@ -12536,8 +12536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{248AD32E-0F60-4FDB-B981-8C15BAA8D65A}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12570,8 +12570,8 @@
         <v>0.19776397684295052</v>
       </c>
       <c r="C2">
-        <f>Sheet1!$G$60</f>
-        <v>0.19776397684295052</v>
+        <f>Sheet1!$G$79</f>
+        <v>0.13851325060502259</v>
       </c>
       <c r="D2">
         <f>Sheet1!$G$69</f>
@@ -12587,8 +12587,8 @@
         <v>0.19776397684295052</v>
       </c>
       <c r="C3">
-        <f>Sheet1!$G$60</f>
-        <v>0.19776397684295052</v>
+        <f>Sheet1!$G$79</f>
+        <v>0.13851325060502259</v>
       </c>
       <c r="D3">
         <f>Sheet1!$G$69</f>
@@ -12604,8 +12604,8 @@
         <v>0.19776397684295052</v>
       </c>
       <c r="C4">
-        <f>Sheet1!$G$60</f>
-        <v>0.19776397684295052</v>
+        <f>Sheet1!$G$79</f>
+        <v>0.13851325060502259</v>
       </c>
       <c r="D4">
         <f>Sheet1!$G$69</f>
@@ -12621,8 +12621,8 @@
         <v>0.19776397684295052</v>
       </c>
       <c r="C5">
-        <f>Sheet1!$G$60</f>
-        <v>0.19776397684295052</v>
+        <f>Sheet1!$G$79</f>
+        <v>0.13851325060502259</v>
       </c>
       <c r="D5">
         <f>Sheet1!$G$69</f>
@@ -12638,8 +12638,8 @@
         <v>0.19776397684295052</v>
       </c>
       <c r="C6">
-        <f>Sheet1!$G$60</f>
-        <v>0.19776397684295052</v>
+        <f>Sheet1!$G$79</f>
+        <v>0.13851325060502259</v>
       </c>
       <c r="D6">
         <f>Sheet1!$G$69</f>
@@ -12655,8 +12655,8 @@
         <v>0.19776397684295052</v>
       </c>
       <c r="C7">
-        <f>Sheet1!$G$60</f>
-        <v>0.19776397684295052</v>
+        <f>Sheet1!$G$79</f>
+        <v>0.13851325060502259</v>
       </c>
       <c r="D7">
         <f>Sheet1!$G$69</f>
@@ -12672,8 +12672,8 @@
         <v>0.19776397684295052</v>
       </c>
       <c r="C8">
-        <f>Sheet1!$G$60</f>
-        <v>0.19776397684295052</v>
+        <f>Sheet1!$G$79</f>
+        <v>0.13851325060502259</v>
       </c>
       <c r="D8">
         <f>Sheet1!$G$69</f>
@@ -12689,8 +12689,8 @@
         <v>0.19776397684295052</v>
       </c>
       <c r="C9">
-        <f>Sheet1!$G$60</f>
-        <v>0.19776397684295052</v>
+        <f>Sheet1!$G$79</f>
+        <v>0.13851325060502259</v>
       </c>
       <c r="D9">
         <f>Sheet1!$G$69</f>
@@ -12706,8 +12706,8 @@
         <v>0.19776397684295052</v>
       </c>
       <c r="C10">
-        <f>Sheet1!$G$60</f>
-        <v>0.19776397684295052</v>
+        <f>Sheet1!$G$79</f>
+        <v>0.13851325060502259</v>
       </c>
       <c r="D10">
         <f>Sheet1!$G$69</f>
@@ -12723,8 +12723,8 @@
         <v>0.19776397684295052</v>
       </c>
       <c r="C11">
-        <f>Sheet1!$G$60</f>
-        <v>0.19776397684295052</v>
+        <f>Sheet1!$G$79</f>
+        <v>0.13851325060502259</v>
       </c>
       <c r="D11">
         <f>Sheet1!$G$69</f>
@@ -12740,8 +12740,8 @@
         <v>0.19776397684295052</v>
       </c>
       <c r="C12">
-        <f>Sheet1!$G$60</f>
-        <v>0.19776397684295052</v>
+        <f>Sheet1!$G$79</f>
+        <v>0.13851325060502259</v>
       </c>
       <c r="D12">
         <f>Sheet1!$G$69</f>
@@ -12757,8 +12757,8 @@
         <v>0.19776397684295052</v>
       </c>
       <c r="C13">
-        <f>Sheet1!$G$60</f>
-        <v>0.19776397684295052</v>
+        <f>Sheet1!$G$79</f>
+        <v>0.13851325060502259</v>
       </c>
       <c r="D13">
         <f>Sheet1!$G$69</f>
@@ -12774,8 +12774,8 @@
         <v>0.19776397684295052</v>
       </c>
       <c r="C14">
-        <f>Sheet1!$G$60</f>
-        <v>0.19776397684295052</v>
+        <f>Sheet1!$G$79</f>
+        <v>0.13851325060502259</v>
       </c>
       <c r="D14">
         <f>Sheet1!$G$69</f>
@@ -12791,8 +12791,8 @@
         <v>0.19776397684295052</v>
       </c>
       <c r="C15">
-        <f>Sheet1!$G$60</f>
-        <v>0.19776397684295052</v>
+        <f>Sheet1!$G$79</f>
+        <v>0.13851325060502259</v>
       </c>
       <c r="D15">
         <f>Sheet1!$G$69</f>
@@ -12808,8 +12808,8 @@
         <v>0.19776397684295052</v>
       </c>
       <c r="C16">
-        <f>Sheet1!$G$60</f>
-        <v>0.19776397684295052</v>
+        <f>Sheet1!$G$79</f>
+        <v>0.13851325060502259</v>
       </c>
       <c r="D16">
         <f>Sheet1!$G$69</f>
@@ -12825,8 +12825,8 @@
         <v>0.19776397684295052</v>
       </c>
       <c r="C17">
-        <f>Sheet1!$G$60</f>
-        <v>0.19776397684295052</v>
+        <f>Sheet1!$G$79</f>
+        <v>0.13851325060502259</v>
       </c>
       <c r="D17">
         <f>Sheet1!$G$69</f>
@@ -12842,8 +12842,8 @@
         <v>0.19776397684295052</v>
       </c>
       <c r="C18">
-        <f>Sheet1!$G$60</f>
-        <v>0.19776397684295052</v>
+        <f>Sheet1!$G$79</f>
+        <v>0.13851325060502259</v>
       </c>
       <c r="D18">
         <f>Sheet1!$G$69</f>
@@ -12859,8 +12859,8 @@
         <v>0.19776397684295052</v>
       </c>
       <c r="C19">
-        <f>Sheet1!$G$60</f>
-        <v>0.19776397684295052</v>
+        <f>Sheet1!$G$79</f>
+        <v>0.13851325060502259</v>
       </c>
       <c r="D19">
         <f>Sheet1!$G$69</f>
@@ -12876,8 +12876,8 @@
         <v>0.19776397684295052</v>
       </c>
       <c r="C20">
-        <f>Sheet1!$G$60</f>
-        <v>0.19776397684295052</v>
+        <f>Sheet1!$G$79</f>
+        <v>0.13851325060502259</v>
       </c>
       <c r="D20">
         <f>Sheet1!$G$69</f>
@@ -12893,8 +12893,8 @@
         <v>0.19776397684295052</v>
       </c>
       <c r="C21">
-        <f>Sheet1!$G$60</f>
-        <v>0.19776397684295052</v>
+        <f>Sheet1!$G$79</f>
+        <v>0.13851325060502259</v>
       </c>
       <c r="D21">
         <f>Sheet1!$G$69</f>
@@ -12910,8 +12910,8 @@
         <v>0.19776397684295052</v>
       </c>
       <c r="C22">
-        <f>Sheet1!$G$60</f>
-        <v>0.19776397684295052</v>
+        <f>Sheet1!$G$79</f>
+        <v>0.13851325060502259</v>
       </c>
       <c r="D22">
         <f>Sheet1!$G$69</f>
@@ -12927,8 +12927,8 @@
         <v>0.19776397684295052</v>
       </c>
       <c r="C23">
-        <f>Sheet1!$G$60</f>
-        <v>0.19776397684295052</v>
+        <f>Sheet1!$G$79</f>
+        <v>0.13851325060502259</v>
       </c>
       <c r="D23">
         <f>Sheet1!$G$69</f>
@@ -12944,8 +12944,8 @@
         <v>0.19776397684295052</v>
       </c>
       <c r="C24">
-        <f>Sheet1!$G$60</f>
-        <v>0.19776397684295052</v>
+        <f>Sheet1!$G$79</f>
+        <v>0.13851325060502259</v>
       </c>
       <c r="D24">
         <f>Sheet1!$G$69</f>
@@ -12961,8 +12961,8 @@
         <v>0.19776397684295052</v>
       </c>
       <c r="C25">
-        <f>Sheet1!$G$60</f>
-        <v>0.19776397684295052</v>
+        <f>Sheet1!$G$79</f>
+        <v>0.13851325060502259</v>
       </c>
       <c r="D25">
         <f>Sheet1!$G$69</f>
@@ -12978,8 +12978,8 @@
         <v>0.19776397684295052</v>
       </c>
       <c r="C26">
-        <f>Sheet1!$G$60</f>
-        <v>0.19776397684295052</v>
+        <f>Sheet1!$G$79</f>
+        <v>0.13851325060502259</v>
       </c>
       <c r="D26">
         <f>Sheet1!$G$69</f>
@@ -12995,8 +12995,8 @@
         <v>0.19776397684295052</v>
       </c>
       <c r="C27">
-        <f>Sheet1!$G$60</f>
-        <v>0.19776397684295052</v>
+        <f>Sheet1!$G$79</f>
+        <v>0.13851325060502259</v>
       </c>
       <c r="D27">
         <f>Sheet1!$G$69</f>
@@ -13012,8 +13012,8 @@
         <v>0.19776397684295052</v>
       </c>
       <c r="C28">
-        <f>Sheet1!$G$60</f>
-        <v>0.19776397684295052</v>
+        <f>Sheet1!$G$79</f>
+        <v>0.13851325060502259</v>
       </c>
       <c r="D28">
         <f>Sheet1!$G$69</f>
@@ -13029,8 +13029,8 @@
         <v>0.19776397684295052</v>
       </c>
       <c r="C29">
-        <f>Sheet1!$G$60</f>
-        <v>0.19776397684295052</v>
+        <f>Sheet1!$G$79</f>
+        <v>0.13851325060502259</v>
       </c>
       <c r="D29">
         <f>Sheet1!$G$69</f>
@@ -13046,8 +13046,8 @@
         <v>0.19776397684295052</v>
       </c>
       <c r="C30">
-        <f>Sheet1!$G$60</f>
-        <v>0.19776397684295052</v>
+        <f>Sheet1!$G$79</f>
+        <v>0.13851325060502259</v>
       </c>
       <c r="D30">
         <f>Sheet1!$G$69</f>
@@ -13063,8 +13063,8 @@
         <v>0.19776397684295052</v>
       </c>
       <c r="C31">
-        <f>Sheet1!$G$60</f>
-        <v>0.19776397684295052</v>
+        <f>Sheet1!$G$79</f>
+        <v>0.13851325060502259</v>
       </c>
       <c r="D31">
         <f>Sheet1!$G$69</f>
@@ -13081,7 +13081,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="C2" sqref="C2:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13114,8 +13114,8 @@
         <v>0.19576110453484274</v>
       </c>
       <c r="C2">
-        <f>Sheet1!$H$60</f>
-        <v>0.19576110453484274</v>
+        <f>Sheet1!$H$79</f>
+        <v>0.14843990302154086</v>
       </c>
       <c r="D2">
         <f>Sheet1!$H$69</f>
@@ -13131,8 +13131,8 @@
         <v>0.19576110453484274</v>
       </c>
       <c r="C3">
-        <f>Sheet1!$H$60</f>
-        <v>0.19576110453484274</v>
+        <f>Sheet1!$H$79</f>
+        <v>0.14843990302154086</v>
       </c>
       <c r="D3">
         <f>Sheet1!$H$69</f>
@@ -13148,8 +13148,8 @@
         <v>0.19576110453484274</v>
       </c>
       <c r="C4">
-        <f>Sheet1!$H$60</f>
-        <v>0.19576110453484274</v>
+        <f>Sheet1!$H$79</f>
+        <v>0.14843990302154086</v>
       </c>
       <c r="D4">
         <f>Sheet1!$H$69</f>
@@ -13165,8 +13165,8 @@
         <v>0.19576110453484274</v>
       </c>
       <c r="C5">
-        <f>Sheet1!$H$60</f>
-        <v>0.19576110453484274</v>
+        <f>Sheet1!$H$79</f>
+        <v>0.14843990302154086</v>
       </c>
       <c r="D5">
         <f>Sheet1!$H$69</f>
@@ -13182,8 +13182,8 @@
         <v>0.19576110453484274</v>
       </c>
       <c r="C6">
-        <f>Sheet1!$H$60</f>
-        <v>0.19576110453484274</v>
+        <f>Sheet1!$H$79</f>
+        <v>0.14843990302154086</v>
       </c>
       <c r="D6">
         <f>Sheet1!$H$69</f>
@@ -13199,8 +13199,8 @@
         <v>0.19576110453484274</v>
       </c>
       <c r="C7">
-        <f>Sheet1!$H$60</f>
-        <v>0.19576110453484274</v>
+        <f>Sheet1!$H$79</f>
+        <v>0.14843990302154086</v>
       </c>
       <c r="D7">
         <f>Sheet1!$H$69</f>
@@ -13216,8 +13216,8 @@
         <v>0.19576110453484274</v>
       </c>
       <c r="C8">
-        <f>Sheet1!$H$60</f>
-        <v>0.19576110453484274</v>
+        <f>Sheet1!$H$79</f>
+        <v>0.14843990302154086</v>
       </c>
       <c r="D8">
         <f>Sheet1!$H$69</f>
@@ -13233,8 +13233,8 @@
         <v>0.19576110453484274</v>
       </c>
       <c r="C9">
-        <f>Sheet1!$H$60</f>
-        <v>0.19576110453484274</v>
+        <f>Sheet1!$H$79</f>
+        <v>0.14843990302154086</v>
       </c>
       <c r="D9">
         <f>Sheet1!$H$69</f>
@@ -13250,8 +13250,8 @@
         <v>0.19576110453484274</v>
       </c>
       <c r="C10">
-        <f>Sheet1!$H$60</f>
-        <v>0.19576110453484274</v>
+        <f>Sheet1!$H$79</f>
+        <v>0.14843990302154086</v>
       </c>
       <c r="D10">
         <f>Sheet1!$H$69</f>
@@ -13267,8 +13267,8 @@
         <v>0.19576110453484274</v>
       </c>
       <c r="C11">
-        <f>Sheet1!$H$60</f>
-        <v>0.19576110453484274</v>
+        <f>Sheet1!$H$79</f>
+        <v>0.14843990302154086</v>
       </c>
       <c r="D11">
         <f>Sheet1!$H$69</f>
@@ -13284,8 +13284,8 @@
         <v>0.19576110453484274</v>
       </c>
       <c r="C12">
-        <f>Sheet1!$H$60</f>
-        <v>0.19576110453484274</v>
+        <f>Sheet1!$H$79</f>
+        <v>0.14843990302154086</v>
       </c>
       <c r="D12">
         <f>Sheet1!$H$69</f>
@@ -13301,8 +13301,8 @@
         <v>0.19576110453484274</v>
       </c>
       <c r="C13">
-        <f>Sheet1!$H$60</f>
-        <v>0.19576110453484274</v>
+        <f>Sheet1!$H$79</f>
+        <v>0.14843990302154086</v>
       </c>
       <c r="D13">
         <f>Sheet1!$H$69</f>
@@ -13318,8 +13318,8 @@
         <v>0.19576110453484274</v>
       </c>
       <c r="C14">
-        <f>Sheet1!$H$60</f>
-        <v>0.19576110453484274</v>
+        <f>Sheet1!$H$79</f>
+        <v>0.14843990302154086</v>
       </c>
       <c r="D14">
         <f>Sheet1!$H$69</f>
@@ -13335,8 +13335,8 @@
         <v>0.19576110453484274</v>
       </c>
       <c r="C15">
-        <f>Sheet1!$H$60</f>
-        <v>0.19576110453484274</v>
+        <f>Sheet1!$H$79</f>
+        <v>0.14843990302154086</v>
       </c>
       <c r="D15">
         <f>Sheet1!$H$69</f>
@@ -13352,8 +13352,8 @@
         <v>0.19576110453484274</v>
       </c>
       <c r="C16">
-        <f>Sheet1!$H$60</f>
-        <v>0.19576110453484274</v>
+        <f>Sheet1!$H$79</f>
+        <v>0.14843990302154086</v>
       </c>
       <c r="D16">
         <f>Sheet1!$H$69</f>
@@ -13369,8 +13369,8 @@
         <v>0.19576110453484274</v>
       </c>
       <c r="C17">
-        <f>Sheet1!$H$60</f>
-        <v>0.19576110453484274</v>
+        <f>Sheet1!$H$79</f>
+        <v>0.14843990302154086</v>
       </c>
       <c r="D17">
         <f>Sheet1!$H$69</f>
@@ -13386,8 +13386,8 @@
         <v>0.19576110453484274</v>
       </c>
       <c r="C18">
-        <f>Sheet1!$H$60</f>
-        <v>0.19576110453484274</v>
+        <f>Sheet1!$H$79</f>
+        <v>0.14843990302154086</v>
       </c>
       <c r="D18">
         <f>Sheet1!$H$69</f>
@@ -13403,8 +13403,8 @@
         <v>0.19576110453484274</v>
       </c>
       <c r="C19">
-        <f>Sheet1!$H$60</f>
-        <v>0.19576110453484274</v>
+        <f>Sheet1!$H$79</f>
+        <v>0.14843990302154086</v>
       </c>
       <c r="D19">
         <f>Sheet1!$H$69</f>
@@ -13420,8 +13420,8 @@
         <v>0.19576110453484274</v>
       </c>
       <c r="C20">
-        <f>Sheet1!$H$60</f>
-        <v>0.19576110453484274</v>
+        <f>Sheet1!$H$79</f>
+        <v>0.14843990302154086</v>
       </c>
       <c r="D20">
         <f>Sheet1!$H$69</f>
@@ -13437,8 +13437,8 @@
         <v>0.19576110453484274</v>
       </c>
       <c r="C21">
-        <f>Sheet1!$H$60</f>
-        <v>0.19576110453484274</v>
+        <f>Sheet1!$H$79</f>
+        <v>0.14843990302154086</v>
       </c>
       <c r="D21">
         <f>Sheet1!$H$69</f>
@@ -13454,8 +13454,8 @@
         <v>0.19576110453484274</v>
       </c>
       <c r="C22">
-        <f>Sheet1!$H$60</f>
-        <v>0.19576110453484274</v>
+        <f>Sheet1!$H$79</f>
+        <v>0.14843990302154086</v>
       </c>
       <c r="D22">
         <f>Sheet1!$H$69</f>
@@ -13471,8 +13471,8 @@
         <v>0.19576110453484274</v>
       </c>
       <c r="C23">
-        <f>Sheet1!$H$60</f>
-        <v>0.19576110453484274</v>
+        <f>Sheet1!$H$79</f>
+        <v>0.14843990302154086</v>
       </c>
       <c r="D23">
         <f>Sheet1!$H$69</f>
@@ -13488,8 +13488,8 @@
         <v>0.19576110453484274</v>
       </c>
       <c r="C24">
-        <f>Sheet1!$H$60</f>
-        <v>0.19576110453484274</v>
+        <f>Sheet1!$H$79</f>
+        <v>0.14843990302154086</v>
       </c>
       <c r="D24">
         <f>Sheet1!$H$69</f>
@@ -13505,8 +13505,8 @@
         <v>0.19576110453484274</v>
       </c>
       <c r="C25">
-        <f>Sheet1!$H$60</f>
-        <v>0.19576110453484274</v>
+        <f>Sheet1!$H$79</f>
+        <v>0.14843990302154086</v>
       </c>
       <c r="D25">
         <f>Sheet1!$H$69</f>
@@ -13522,8 +13522,8 @@
         <v>0.19576110453484274</v>
       </c>
       <c r="C26">
-        <f>Sheet1!$H$60</f>
-        <v>0.19576110453484274</v>
+        <f>Sheet1!$H$79</f>
+        <v>0.14843990302154086</v>
       </c>
       <c r="D26">
         <f>Sheet1!$H$69</f>
@@ -13539,8 +13539,8 @@
         <v>0.19576110453484274</v>
       </c>
       <c r="C27">
-        <f>Sheet1!$H$60</f>
-        <v>0.19576110453484274</v>
+        <f>Sheet1!$H$79</f>
+        <v>0.14843990302154086</v>
       </c>
       <c r="D27">
         <f>Sheet1!$H$69</f>
@@ -13556,8 +13556,8 @@
         <v>0.19576110453484274</v>
       </c>
       <c r="C28">
-        <f>Sheet1!$H$60</f>
-        <v>0.19576110453484274</v>
+        <f>Sheet1!$H$79</f>
+        <v>0.14843990302154086</v>
       </c>
       <c r="D28">
         <f>Sheet1!$H$69</f>
@@ -13573,8 +13573,8 @@
         <v>0.19576110453484274</v>
       </c>
       <c r="C29">
-        <f>Sheet1!$H$60</f>
-        <v>0.19576110453484274</v>
+        <f>Sheet1!$H$79</f>
+        <v>0.14843990302154086</v>
       </c>
       <c r="D29">
         <f>Sheet1!$H$69</f>
@@ -13590,8 +13590,8 @@
         <v>0.19576110453484274</v>
       </c>
       <c r="C30">
-        <f>Sheet1!$H$60</f>
-        <v>0.19576110453484274</v>
+        <f>Sheet1!$H$79</f>
+        <v>0.14843990302154086</v>
       </c>
       <c r="D30">
         <f>Sheet1!$H$69</f>
@@ -13607,8 +13607,8 @@
         <v>0.19576110453484274</v>
       </c>
       <c r="C31">
-        <f>Sheet1!$H$60</f>
-        <v>0.19576110453484274</v>
+        <f>Sheet1!$H$79</f>
+        <v>0.14843990302154086</v>
       </c>
       <c r="D31">
         <f>Sheet1!$H$69</f>

</xml_diff>